<commit_message>
Source files now work.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0566EB63-585C-4762-B550-6D622C1FEF96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653B0DAB-E826-4B22-99B2-BF28590447E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14235" yWindow="-16425" windowWidth="29040" windowHeight="15840" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -479,7 +479,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -546,7 +546,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -555,16 +555,16 @@
         <v>4</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <f>B4*C4/D4</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -582,43 +582,43 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
+        <v>8</v>
+      </c>
+      <c r="B6" s="3">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <f>B6*C6/D6</f>
-        <v>0.8</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="3">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <f>B7*C7/D7</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -627,47 +627,47 @@
         <v>2</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E8">
         <f>B8*C8/D8</f>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E9">
         <f>B9*C9/D9</f>
-        <v>0.4</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <f>B10*C10/D10</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
HP complete and MANIFEST.in included.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson\PycharmProjects\hs-logger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8686D656-4547-4F60-B77F-D9DE03E1AFF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BA6790-3660-480F-BB3B-D0709C980EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>Mensor CPT9000</t>
+  </si>
+  <si>
+    <t>Fix datafile filenames</t>
   </si>
 </sst>
 </file>
@@ -506,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875FA9E-03C5-44EF-91A8-26A2DEEA24CC}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -540,7 +543,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -549,16 +552,16 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <f>B2*C2/D2</f>
-        <v>2</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -576,7 +579,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -594,7 +597,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -612,70 +615,70 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <f>B6*C6/D6</f>
-        <v>1.3333333333333333</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="1">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2">
         <v>1</v>
       </c>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7">
         <f>B7*C7/D7</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2">
         <v>1</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8">
         <f>B8*C8/D8</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="2">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9">
         <f>B9*C9/D9</f>
@@ -683,17 +686,17 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <f>B10*C10/D10</f>
@@ -702,63 +705,63 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <f>B11*C11/D11</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="1">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3">
         <v>1</v>
       </c>
       <c r="C12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D12">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12">
         <f>B12*C12/D12</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f>B13*C13/D13</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="3">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14">
@@ -774,7 +777,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -783,97 +786,97 @@
         <v>2</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15">
         <f>B15*C15/D15</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="B16" s="2">
         <v>1</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16">
         <f>B16*C16/D16</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E17">
         <f>B17*C17/D17</f>
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E18">
         <f>B18*C18/D18</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="2">
-        <v>1</v>
+        <v>26</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>3</v>
       </c>
       <c r="E19">
         <f>B19*C19/D19</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E20">
         <f>B20*C20/D20</f>
@@ -882,7 +885,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -891,7 +894,7 @@
         <v>4</v>
       </c>
       <c r="D21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21">
         <f>B21*C21/D21</f>
@@ -900,7 +903,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -909,7 +912,7 @@
         <v>4</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E22">
         <f>B22*C22/D22</f>
@@ -918,13 +921,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
       <c r="C23">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -936,16 +939,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
         <f>B24*C24/D24</f>
@@ -954,7 +957,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -972,16 +975,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26">
         <f>B26*C26/D26</f>
@@ -990,16 +993,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27">
         <f>B27*C27/D27</f>
@@ -1008,16 +1011,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28">
         <f>B28*C28/D28</f>
@@ -1026,7 +1029,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1044,32 +1047,50 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E30">
         <f>B30*C30/D30</f>
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <f>B31*C31/D31</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E30">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
       <sortCondition descending="1" ref="E1:E13"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
     <sortCondition descending="1" ref="E2:E12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D30">
+  <conditionalFormatting sqref="D2:D31">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1079,7 +1100,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E30">
+  <conditionalFormatting sqref="E2:E31">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1091,7 +1112,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C30">
+  <conditionalFormatting sqref="C2:C31">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Transform toggle and comments added.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BA6790-3660-480F-BB3B-D0709C980EDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226AA265-7464-4732-8268-76B4FB2682AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Fix datafile filenames</t>
+  </si>
+  <si>
+    <t>Add references</t>
   </si>
 </sst>
 </file>
@@ -183,15 +186,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875FA9E-03C5-44EF-91A8-26A2DEEA24CC}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B15" sqref="B15:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -615,7 +615,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -624,11 +624,11 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6">
         <f>B6*C6/D6</f>
-        <v>1.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -650,7 +650,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2">
@@ -687,45 +687,45 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <f>B10*C10/D10</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11">
         <f>B11*C11/D11</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="3">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12">
@@ -741,7 +741,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -750,76 +750,76 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E13">
         <f>B13*C13/D13</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="1">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14">
         <f>B14*C14/D14</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15">
         <f>B15*C15/D15</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <f>B16*C16/D16</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>2</v>
@@ -831,16 +831,16 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18">
         <f>B18*C18/D18</f>
@@ -849,7 +849,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -858,7 +858,7 @@
         <v>4</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E19">
         <f>B19*C19/D19</f>
@@ -867,7 +867,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -876,7 +876,7 @@
         <v>2</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20">
         <f>B20*C20/D20</f>
@@ -885,16 +885,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E21">
         <f>B21*C21/D21</f>
@@ -903,7 +903,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -930,7 +930,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E23">
         <f>B23*C23/D23</f>
@@ -939,16 +939,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E24">
         <f>B24*C24/D24</f>
@@ -957,16 +957,16 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
       <c r="C25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E25">
         <f>B25*C25/D25</f>
@@ -975,16 +975,16 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26">
         <f>B26*C26/D26</f>
@@ -993,16 +993,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E27">
         <f>B27*C27/D27</f>
@@ -1011,16 +1011,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
       <c r="C28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E28">
         <f>B28*C28/D28</f>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1038,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E29">
         <f>B29*C29/D29</f>
@@ -1047,16 +1047,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E30">
         <f>B30*C30/D30</f>
@@ -1065,32 +1065,50 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31">
         <f>B31*C31/D31</f>
         <v>0</v>
       </c>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <f>B32*C32/D32</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E32">
       <sortCondition descending="1" ref="E1:E13"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
     <sortCondition descending="1" ref="E2:E12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D31">
+  <conditionalFormatting sqref="D2:D32">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1100,7 +1118,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E31">
+  <conditionalFormatting sqref="E2:E32">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1112,7 +1130,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C31">
+  <conditionalFormatting sqref="C2:C32">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1134,7 +1152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B30">
+  <conditionalFormatting sqref="B2:B32">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Fixed hanging issue and started implementation of references.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226AA265-7464-4732-8268-76B4FB2682AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50D4918-1C15-4D07-B4E6-6902348DEBAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Add references</t>
+  </si>
+  <si>
+    <t>Print current point on screen</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875FA9E-03C5-44EF-91A8-26A2DEEA24CC}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B32"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,7 +690,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -696,34 +699,34 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f>B10*C10/D10</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <f>B11*C11/D11</f>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -741,7 +744,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -750,58 +753,58 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f>B13*C13/D13</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <f>B14*C14/D14</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <f>B15*C15/D15</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -813,16 +816,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <f>B17*C17/D17</f>
@@ -831,7 +834,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -849,13 +852,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -867,16 +870,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <f>B20*C20/D20</f>
@@ -885,16 +888,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f>B21*C21/D21</f>
@@ -903,16 +906,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <f>B22*C22/D22</f>
@@ -921,7 +924,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -939,7 +942,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -957,7 +960,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -975,7 +978,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -993,16 +996,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <f>B27*C27/D27</f>
@@ -1011,7 +1014,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1029,13 +1032,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -1047,13 +1050,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -1065,16 +1068,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <f>B31*C31/D31</f>
@@ -1083,7 +1086,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1099,16 +1102,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <f>B33*C33/D33</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E32">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E33">
       <sortCondition descending="1" ref="E1:E13"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
     <sortCondition descending="1" ref="E2:E12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1118,7 +1139,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E32">
+  <conditionalFormatting sqref="E2:E33">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1130,7 +1151,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C32">
+  <conditionalFormatting sqref="C2:C33">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
New instrument files & fixed labels.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226AA265-7464-4732-8268-76B4FB2682AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50D4918-1C15-4D07-B4E6-6902348DEBAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Add references</t>
+  </si>
+  <si>
+    <t>Print current point on screen</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875FA9E-03C5-44EF-91A8-26A2DEEA24CC}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B32"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -687,7 +690,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -696,34 +699,34 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10">
         <f>B10*C10/D10</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11">
         <f>B11*C11/D11</f>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -741,7 +744,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -750,58 +753,58 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13">
         <f>B13*C13/D13</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14">
         <f>B14*C14/D14</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15">
         <f>B15*C15/D15</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -813,16 +816,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
         <f>B17*C17/D17</f>
@@ -831,7 +834,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -849,13 +852,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -867,16 +870,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20">
         <f>B20*C20/D20</f>
@@ -885,16 +888,16 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
       <c r="C21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f>B21*C21/D21</f>
@@ -903,16 +906,16 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22">
         <f>B22*C22/D22</f>
@@ -921,7 +924,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -939,7 +942,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -957,7 +960,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -975,7 +978,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -993,16 +996,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E27">
         <f>B27*C27/D27</f>
@@ -1011,7 +1014,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1029,13 +1032,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -1047,13 +1050,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30">
         <v>4</v>
@@ -1065,16 +1068,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31">
         <f>B31*C31/D31</f>
@@ -1083,7 +1086,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1099,16 +1102,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33">
+        <f>B33*C33/D33</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E13" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E32">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E33">
       <sortCondition descending="1" ref="E1:E13"/>
     </sortState>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
     <sortCondition descending="1" ref="E2:E12"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D32">
+  <conditionalFormatting sqref="D2:D33">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1118,7 +1139,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E32">
+  <conditionalFormatting sqref="E2:E33">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1130,7 +1151,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C32">
+  <conditionalFormatting sqref="C2:C33">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
References can now be used.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B234C6ED-328F-4D5A-98FF-190FDA15AC58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E03D9B-F52D-48CE-8D30-2A2154FE10F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -585,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <f>B2*C2/D2</f>
+        <f t="shared" ref="E2:E42" si="0">B2*C2/D2</f>
         <v>2</v>
       </c>
     </row>
@@ -603,7 +604,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f>B3*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -621,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <f>B4*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -639,7 +640,7 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <f>B5*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -657,7 +658,7 @@
         <v>3</v>
       </c>
       <c r="E6">
-        <f>B6*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -675,7 +676,7 @@
         <v>3</v>
       </c>
       <c r="E7">
-        <f>B7*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -693,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="E8">
-        <f>B8*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -711,7 +712,7 @@
         <v>3</v>
       </c>
       <c r="E9">
-        <f>B9*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -729,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <f>B10*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -747,7 +748,7 @@
         <v>2</v>
       </c>
       <c r="E11">
-        <f>B11*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -765,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="E12">
-        <f>B12*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
     </row>
@@ -783,7 +784,7 @@
         <v>4</v>
       </c>
       <c r="E13">
-        <f>B13*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
     </row>
@@ -801,7 +802,7 @@
         <v>3</v>
       </c>
       <c r="E14">
-        <f>B14*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -819,7 +820,7 @@
         <v>3</v>
       </c>
       <c r="E15">
-        <f>B15*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -837,7 +838,7 @@
         <v>3</v>
       </c>
       <c r="E16">
-        <f>B16*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -855,7 +856,7 @@
         <v>3</v>
       </c>
       <c r="E17">
-        <f>B17*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -873,7 +874,7 @@
         <v>4</v>
       </c>
       <c r="E18">
-        <f>B18*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -891,7 +892,7 @@
         <v>3</v>
       </c>
       <c r="E19">
-        <f>B19*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -909,7 +910,7 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <f>B20*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -927,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <f>B21*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -945,7 +946,7 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <f>B22*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -963,7 +964,7 @@
         <v>1</v>
       </c>
       <c r="E23">
-        <f>B23*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -981,7 +982,7 @@
         <v>1</v>
       </c>
       <c r="E24">
-        <f>B24*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -999,7 +1000,7 @@
         <v>2</v>
       </c>
       <c r="E25">
-        <f>B25*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1017,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="E26">
-        <f>B26*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1035,7 +1036,7 @@
         <v>2</v>
       </c>
       <c r="E27">
-        <f>B27*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1053,7 +1054,7 @@
         <v>2</v>
       </c>
       <c r="E28">
-        <f>B28*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1071,7 +1072,7 @@
         <v>3</v>
       </c>
       <c r="E29">
-        <f>B29*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1089,7 +1090,7 @@
         <v>3</v>
       </c>
       <c r="E30">
-        <f>B30*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1107,7 +1108,7 @@
         <v>3</v>
       </c>
       <c r="E31">
-        <f>B31*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1125,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="E32">
-        <f>B32*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1143,7 +1144,7 @@
         <v>3</v>
       </c>
       <c r="E33">
-        <f>B33*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1161,7 +1162,7 @@
         <v>3</v>
       </c>
       <c r="E34">
-        <f>B34*C34/D34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1179,7 +1180,7 @@
         <v>3</v>
       </c>
       <c r="E35">
-        <f>B35*C35/D35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1197,7 +1198,7 @@
         <v>3</v>
       </c>
       <c r="E36">
-        <f>B36*C36/D36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1215,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="E37">
-        <f>B37*C37/D37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1233,7 +1234,7 @@
         <v>4</v>
       </c>
       <c r="E38">
-        <f>B38*C38/D38</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1251,7 +1252,7 @@
         <v>4</v>
       </c>
       <c r="E39">
-        <f>B39*C39/D39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1269,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <f>B40*C40/D40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1287,7 +1288,7 @@
         <v>4</v>
       </c>
       <c r="E41">
-        <f>B41*C41/D41</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1305,7 +1306,7 @@
         <v>3</v>
       </c>
       <c r="E42">
-        <f>B42*C42/D42</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ease of use fixes.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D8F14D-0EF6-4E7B-A17E-1C9F04EDBCE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084C7E0D-2EAA-4A21-B1C7-BF4F0D479593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2640" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Graph transforms</t>
   </si>
   <si>
-    <t>Last/next N button</t>
-  </si>
-  <si>
     <t>Report #s and dates</t>
   </si>
   <si>
@@ -175,13 +172,31 @@
   </si>
   <si>
     <t>Graph names</t>
+  </si>
+  <si>
+    <t>Check setpoints are set</t>
+  </si>
+  <si>
+    <t>Autoprofile controls</t>
+  </si>
+  <si>
+    <t>Scroll bar issues</t>
+  </si>
+  <si>
+    <t>Mensor measurement E issue</t>
+  </si>
+  <si>
+    <t>Freeze if point moves during scroll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +209,19 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +253,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875FA9E-03C5-44EF-91A8-26A2DEEA24CC}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -551,7 +582,7 @@
     <col min="2" max="2" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -572,111 +603,111 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>36</v>
+      <c r="A2" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
         <f>B2*C2/D2</f>
-        <v>1.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>44</v>
+      <c r="A3" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="6">
         <f>B3*C3/D3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="6">
+        <f>B4*C4/D4</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <f>B5*C5/D5</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
-      </c>
-      <c r="E4">
-        <f>B4*C4/D4</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5">
-        <f>B5*C5/D5</f>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6">
+        <f>B6*C6/D6</f>
         <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <f>B6*C6/D6</f>
-        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="6">
         <f>B7*C7/D7</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -692,68 +723,68 @@
       <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="6">
         <f>B8*C8/D8</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="E9" s="6">
         <f>B9*C9/D9</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <f>B10*C10/D10</f>
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6">
         <f>B11*C11/D11</f>
-        <v>0.66666666666666663</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -764,14 +795,14 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="6">
         <f>B12*C12/D12</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -782,14 +813,14 @@
       <c r="D13">
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="6">
         <f>B13*C13/D13</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -798,55 +829,55 @@
         <v>2</v>
       </c>
       <c r="D14">
-        <v>4</v>
-      </c>
-      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="6">
         <f>B14*C14/D14</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="2">
+        <v>18</v>
+      </c>
+      <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="E15" s="6">
         <f>B15*C15/D15</f>
-        <v>0.33333333333333331</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
       </c>
       <c r="C16">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
-      </c>
-      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="E16" s="6">
         <f>B16*C16/D16</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C17">
         <v>5</v>
@@ -854,215 +885,215 @@
       <c r="D17">
         <v>1</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="6">
         <f>B17*C17/D17</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C18">
         <v>5</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="6">
         <f>B18*C18/D18</f>
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6">
         <f>B19*C19/D19</f>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>4</v>
-      </c>
-      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
         <f>B20*C20/D20</f>
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="6">
         <f>B21*C21/D21</f>
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C22">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="6">
         <f>B22*C22/D22</f>
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B23" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D23">
-        <v>1</v>
-      </c>
-      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="E23" s="6">
         <f>B23*C23/D23</f>
-        <v>0</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B24" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D24">
-        <v>2</v>
-      </c>
-      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="E24" s="6">
         <f>B24*C24/D24</f>
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="E25" s="6">
         <f>B25*C25/D25</f>
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>28</v>
+      <c r="A26" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26">
-        <v>3</v>
-      </c>
-      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="E26" s="6">
         <f>B26*C26/D26</f>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>27</v>
+      <c r="A27" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="B27" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27">
-        <v>3</v>
-      </c>
-      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="E27" s="6">
         <f>B27*C27/D27</f>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B28" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C28">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>3</v>
-      </c>
-      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="6">
         <f>B28*C28/D28</f>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B29" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -1070,17 +1101,17 @@
       <c r="D29">
         <v>3</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="6">
         <f>B29*C29/D29</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -1088,17 +1119,17 @@
       <c r="D30">
         <v>3</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="6">
         <f>B30*C30/D30</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C31">
         <v>4</v>
@@ -1106,17 +1137,17 @@
       <c r="D31">
         <v>3</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="6">
         <f>B31*C31/D31</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B32" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -1124,17 +1155,17 @@
       <c r="D32">
         <v>3</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="6">
         <f>B32*C32/D32</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B33" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1142,17 +1173,17 @@
       <c r="D33">
         <v>3</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="6">
         <f>B33*C33/D33</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C34">
         <v>4</v>
@@ -1160,176 +1191,250 @@
       <c r="D34">
         <v>3</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="6">
         <f>B34*C34/D34</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B35" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35">
-        <v>4</v>
-      </c>
-      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="E35" s="6">
         <f>B35*C35/D35</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B36" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
       <c r="D36">
-        <v>4</v>
-      </c>
-      <c r="E36">
+        <v>3</v>
+      </c>
+      <c r="E36" s="6">
         <f>B36*C36/D36</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
+        <v>3</v>
+      </c>
+      <c r="E37" s="6">
         <f>B37*C37/D37</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38">
-        <v>2</v>
-      </c>
-      <c r="E38">
+        <v>3</v>
+      </c>
+      <c r="E38" s="6">
         <f>B38*C38/D38</f>
-        <v>0</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="B39" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D39">
         <v>4</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="6">
         <f>B39*C39/D39</f>
-        <v>0</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="B40" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D40">
         <v>4</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="6">
         <f>B40*C40/D40</f>
-        <v>0</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B41" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="E41" s="6">
         <f>B41*C41/D41</f>
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B42" s="1">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42" s="6">
+        <f>B42*C42/D42</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+      <c r="D43">
+        <v>4</v>
+      </c>
+      <c r="E43" s="6">
+        <f>B43*C43/D43</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>34</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>4</v>
+      </c>
+      <c r="E44" s="6">
+        <f>B44*C44/D44</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45" s="6">
+        <f>B45*C45/D45</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C46">
         <v>2</v>
       </c>
-      <c r="D42">
-        <v>3</v>
-      </c>
-      <c r="E42">
-        <f>B42*C42/D42</f>
-        <v>0</v>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46" s="6">
+        <f>B46*C46/D46</f>
+        <v>6.6666666666666671E-3</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E13" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E42">
-      <sortCondition descending="1" ref="E1:E13"/>
+  <autoFilter ref="A1:E12" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E46">
+      <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
-    <sortCondition descending="1" ref="E2:E12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
+    <sortCondition descending="1" ref="E2:E11"/>
   </sortState>
-  <conditionalFormatting sqref="D2:D36">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C33">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="D36:D46">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1338,8 +1443,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="C33:C46">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1349,71 +1464,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B32">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E42">
-    <cfRule type="colorScale" priority="40">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D37:D42">
-    <cfRule type="colorScale" priority="45">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C42">
-    <cfRule type="colorScale" priority="47">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C42">
     <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D42">
-    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1582,18 +1633,70 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B41">
+  <conditionalFormatting sqref="D2:D37">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C32">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B31">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E46">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C46">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D46">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
Append/deete graphs added 2500/2900/3900 standardized Mensor hopefully fixed
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mandy\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084C7E0D-2EAA-4A21-B1C7-BF4F0D479593}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -187,14 +186,17 @@
   </si>
   <si>
     <t>Freeze if point moves during scroll</t>
+  </si>
+  <si>
+    <t>Autoprofile actions</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -255,7 +257,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,23 +571,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875FA9E-03C5-44EF-91A8-26A2DEEA24CC}">
-  <dimension ref="A1:E46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,9 +604,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -613,72 +615,72 @@
         <v>4</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="6">
         <f>B2*C2/D2</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="6">
         <f>B3*C3/D3</f>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
       </c>
       <c r="E4" s="6">
         <f>B4*C4/D4</f>
-        <v>1.6666666666666667</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="2">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="6">
         <f>B5*C5/D5</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2">
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6">
@@ -692,27 +694,27 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>3</v>
       </c>
       <c r="E7" s="6">
         <f>B7*C7/D7</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -728,61 +730,61 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>46</v>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E9" s="6">
         <f>B9*C9/D9</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
       <c r="E10" s="6">
         <f>B10*C10/D10</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" s="6">
         <f>B11*C11/D11</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -800,7 +802,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -818,7 +820,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -836,7 +838,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -854,7 +856,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -872,7 +874,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -890,7 +892,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -908,7 +910,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -926,7 +928,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -944,7 +946,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -962,7 +964,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -980,7 +982,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -998,7 +1000,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1016,7 +1018,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1034,7 +1036,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>43</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>35</v>
       </c>
@@ -1070,7 +1072,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1088,7 +1090,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1106,7 +1108,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1124,7 +1126,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -1142,7 +1144,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1178,7 +1180,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>26</v>
       </c>
@@ -1196,7 +1198,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -1214,7 +1216,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1232,7 +1234,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1268,7 +1270,7 @@
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>19</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1</v>
       </c>
@@ -1304,7 +1306,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -1322,7 +1324,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -1340,7 +1342,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>47</v>
       </c>
@@ -1358,7 +1360,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>34</v>
       </c>
@@ -1376,7 +1378,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1394,7 +1396,7 @@
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -1412,13 +1414,31 @@
         <v>6.6666666666666671E-3</v>
       </c>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C47">
+        <v>4</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" s="6">
+        <f>B47*C47/D47</f>
+        <v>-4</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E12" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E46">
+  <autoFilter ref="A1:E12">
+    <sortState ref="A2:E47">
       <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
+  <sortState ref="A2:E11">
     <sortCondition descending="1" ref="E2:E11"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
@@ -1433,7 +1453,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:D46">
+  <conditionalFormatting sqref="D36:D47">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -1443,7 +1463,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:C46">
+  <conditionalFormatting sqref="C33:C47">
     <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
@@ -1673,7 +1693,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E46">
+  <conditionalFormatting sqref="E2:E47">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -1685,7 +1705,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C46">
+  <conditionalFormatting sqref="C2:C47">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -1695,7 +1715,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D2:D47">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Runtime now correctly starts at 0.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -211,12 +211,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -227,6 +221,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,10 +259,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,9 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -622,7 +620,7 @@
       <c r="D2" s="1">
         <v>2</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <f>B2*C2/D2</f>
         <v>2</v>
       </c>
@@ -640,13 +638,13 @@
       <c r="D3" s="1">
         <v>2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <f>B3*C3/D3</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2">
@@ -658,7 +656,7 @@
       <c r="D4" s="1">
         <v>3</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <f>B4*C4/D4</f>
         <v>1.3333333333333333</v>
       </c>
@@ -676,14 +674,14 @@
       <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <f>B5*C5/D5</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>49</v>
+      <c r="A6" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -694,32 +692,32 @@
       <c r="D6" s="1">
         <v>3</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <f>B6*C6/D6</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>51</v>
+      <c r="A7" t="s">
+        <v>36</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <f>B7*C7/D7</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -730,14 +728,14 @@
       <c r="D8" s="1">
         <v>3</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <f>B8*C8/D8</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -746,34 +744,34 @@
         <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>3</v>
-      </c>
-      <c r="E9" s="6">
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
         <f>B9*C9/D9</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>47</v>
+      <c r="A10" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>4</v>
-      </c>
-      <c r="E10" s="6">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5">
         <f>B10*C10/D10</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>29</v>
+      <c r="A11" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -784,14 +782,14 @@
       <c r="D11" s="1">
         <v>3</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <f>B11*C11/D11</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -802,50 +800,50 @@
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <f>B12*C12/D12</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2">
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <f>B13*C13/D13</f>
-        <v>0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0.01</v>
       </c>
       <c r="C14" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
-        <v>3</v>
-      </c>
-      <c r="E14" s="6">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
         <f>B14*C14/D14</f>
-        <v>0.33333333333333331</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>0.01</v>
@@ -856,32 +854,32 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <f>B15*C15/D15</f>
         <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" s="1">
         <v>0.01</v>
       </c>
       <c r="C16" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="5">
         <f>B16*C16/D16</f>
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="B17" s="1">
         <v>0.01</v>
@@ -892,50 +890,50 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <f>B17*C17/D17</f>
         <v>0.04</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="1">
         <v>0.01</v>
       </c>
       <c r="C18" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <f>B18*C18/D18</f>
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B19" s="1">
         <v>0.01</v>
       </c>
       <c r="C19" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="6">
+        <v>2</v>
+      </c>
+      <c r="E19" s="5">
         <f>B19*C19/D19</f>
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1">
         <v>0.01</v>
@@ -946,68 +944,68 @@
       <c r="D20" s="1">
         <v>2</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <f>B20*C20/D20</f>
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C21" s="1">
         <v>2</v>
       </c>
-      <c r="B21" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C21" s="1">
-        <v>5</v>
-      </c>
       <c r="D21" s="1">
-        <v>2</v>
-      </c>
-      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5">
         <f>B21*C21/D21</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
         <v>0.01</v>
       </c>
       <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
         <v>2</v>
       </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <f>B22*C22/D22</f>
         <v>0.02</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>24</v>
+      <c r="A23" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B23" s="1">
         <v>0.01</v>
       </c>
       <c r="C23" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1">
         <v>2</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <f>B23*C23/D23</f>
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>40</v>
+      <c r="A24" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B24" s="1">
         <v>0.01</v>
@@ -1018,14 +1016,14 @@
       <c r="D24" s="1">
         <v>2</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <f>B24*C24/D24</f>
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>34</v>
+      <c r="A25" t="s">
+        <v>17</v>
       </c>
       <c r="B25" s="1">
         <v>0.01</v>
@@ -1036,32 +1034,32 @@
       <c r="D25" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <f>B25*C25/D25</f>
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1">
         <v>0.01</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
-        <v>2</v>
-      </c>
-      <c r="E26" s="6">
+        <v>3</v>
+      </c>
+      <c r="E26" s="5">
         <f>B26*C26/D26</f>
-        <v>1.4999999999999999E-2</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1">
         <v>0.01</v>
@@ -1072,14 +1070,14 @@
       <c r="D27" s="1">
         <v>3</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <f>B27*C27/D27</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
         <v>0.01</v>
@@ -1090,14 +1088,14 @@
       <c r="D28" s="1">
         <v>3</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <f>B28*C28/D28</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>0.01</v>
@@ -1108,14 +1106,14 @@
       <c r="D29" s="1">
         <v>3</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <f>B29*C29/D29</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B30" s="1">
         <v>0.01</v>
@@ -1126,14 +1124,14 @@
       <c r="D30" s="1">
         <v>3</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <f>B30*C30/D30</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B31" s="1">
         <v>0.01</v>
@@ -1144,14 +1142,14 @@
       <c r="D31" s="1">
         <v>3</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <f>B31*C31/D31</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1">
         <v>0.01</v>
@@ -1162,14 +1160,14 @@
       <c r="D32" s="1">
         <v>3</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <f>B32*C32/D32</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B33" s="1">
         <v>0.01</v>
@@ -1180,14 +1178,14 @@
       <c r="D33" s="1">
         <v>3</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <f>B33*C33/D33</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B34" s="1">
         <v>0.01</v>
@@ -1198,14 +1196,14 @@
       <c r="D34" s="1">
         <v>3</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <f>B34*C34/D34</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B35" s="1">
         <v>0.01</v>
@@ -1216,14 +1214,14 @@
       <c r="D35" s="1">
         <v>3</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <f>B35*C35/D35</f>
         <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>41</v>
+      <c r="A36" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B36" s="1">
         <v>0.01</v>
@@ -1234,7 +1232,7 @@
       <c r="D36" s="1">
         <v>3</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <f>B36*C36/D36</f>
         <v>1.3333333333333334E-2</v>
       </c>
@@ -1252,7 +1250,7 @@
       <c r="D37" s="1">
         <v>4</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <f>B37*C37/D37</f>
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1270,7 +1268,7 @@
       <c r="D38" s="1">
         <v>4</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <f>B38*C38/D38</f>
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1288,7 +1286,7 @@
       <c r="D39" s="1">
         <v>4</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <f>B39*C39/D39</f>
         <v>0.01</v>
       </c>
@@ -1306,50 +1304,50 @@
       <c r="D40" s="1">
         <v>4</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <f>B40*C40/D40</f>
         <v>0.01</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>44</v>
+      <c r="A41" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B41" s="1">
         <v>0.01</v>
       </c>
       <c r="C41" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D41" s="1">
-        <v>4</v>
-      </c>
-      <c r="E41" s="6">
+        <v>5</v>
+      </c>
+      <c r="E41" s="5">
         <f>B41*C41/D41</f>
-        <v>7.4999999999999997E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B42" s="1">
         <v>0.01</v>
       </c>
       <c r="C42" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D42" s="1">
-        <v>4</v>
-      </c>
-      <c r="E42" s="6">
+        <v>5</v>
+      </c>
+      <c r="E42" s="5">
         <f>B42*C42/D42</f>
-        <v>7.4999999999999997E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>21</v>
+      <c r="A43" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B43" s="1">
         <v>0.01</v>
@@ -1360,67 +1358,67 @@
       <c r="D43" s="1">
         <v>4</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <f>B43*C43/D43</f>
         <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B44" s="1">
         <v>0.01</v>
       </c>
       <c r="C44" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1">
-        <v>3</v>
-      </c>
-      <c r="E44" s="6">
+        <v>4</v>
+      </c>
+      <c r="E44" s="5">
         <f>B44*C44/D44</f>
-        <v>6.6666666666666671E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B45" s="1">
-        <v>-1</v>
+        <v>0.01</v>
       </c>
       <c r="C45" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1">
-        <v>5</v>
-      </c>
-      <c r="E45" s="6">
+        <v>4</v>
+      </c>
+      <c r="E45" s="5">
         <f>B45*C45/D45</f>
-        <v>-0.8</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>19</v>
+      <c r="A46" t="s">
+        <v>50</v>
       </c>
       <c r="B46" s="1">
-        <v>-1</v>
+        <v>0.01</v>
       </c>
       <c r="C46" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D46" s="1">
-        <v>5</v>
-      </c>
-      <c r="E46" s="6">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5">
         <f>B46*C46/D46</f>
-        <v>-1</v>
+        <v>6.6666666666666671E-3</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B47" s="1">
@@ -1432,13 +1430,13 @@
       <c r="D47" s="1">
         <v>3</v>
       </c>
-      <c r="E47" s="6">
+      <c r="E47" s="5">
         <f>B47*C47/D47</f>
         <v>-1.6666666666666667</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B48" s="1">
@@ -1450,7 +1448,7 @@
       <c r="D48" s="1">
         <v>1</v>
       </c>
-      <c r="E48" s="6">
+      <c r="E48" s="5">
         <f>B48*C48/D48</f>
         <v>-4</v>
       </c>

</xml_diff>

<commit_message>
Added "time.runtime" safety valve for graphing purposes.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -192,6 +192,27 @@
   </si>
   <si>
     <t>Julabo FP79</t>
+  </si>
+  <si>
+    <t>Cancel load profile</t>
+  </si>
+  <si>
+    <t>Save profile</t>
+  </si>
+  <si>
+    <t>Save points (autoprofile tab)</t>
+  </si>
+  <si>
+    <t>Fix autosize columns?</t>
+  </si>
+  <si>
+    <t>Restart point</t>
+  </si>
+  <si>
+    <t>Reset autoprofile</t>
+  </si>
+  <si>
+    <t>Autoprofile first cell filename</t>
   </si>
 </sst>
 </file>
@@ -577,9 +598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -608,8 +631,8 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>42</v>
+      <c r="A2" t="s">
+        <v>52</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -618,70 +641,70 @@
         <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <f>B2*C2/D2</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>35</v>
+      <c r="A3" t="s">
+        <v>58</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <f>B3*C3/D3</f>
-        <v>1.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
         <f>B4*C4/D4</f>
-        <v>1.3333333333333333</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>3</v>
-      </c>
-      <c r="E5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
         <f>B5*C5/D5</f>
-        <v>1.3333333333333333</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>51</v>
+      <c r="A6" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -690,16 +713,16 @@
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="5">
         <f>B6*C6/D6</f>
-        <v>1.3333333333333333</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>36</v>
+      <c r="A7" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -708,16 +731,16 @@
         <v>3</v>
       </c>
       <c r="D7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" s="5">
         <f>B7*C7/D7</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -726,214 +749,214 @@
         <v>3</v>
       </c>
       <c r="D8" s="1">
-        <v>3</v>
-      </c>
-      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
         <f>B8*C8/D8</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="1">
+      <c r="A9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9" s="5">
         <f>B9*C9/D9</f>
-        <v>0.75</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>29</v>
+      <c r="A10" t="s">
+        <v>46</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="5">
         <f>B10*C10/D10</f>
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="5">
         <f>B11*C11/D11</f>
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1">
         <v>3</v>
       </c>
       <c r="E12" s="5">
         <f>B12*C12/D12</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2">
+        <v>43</v>
+      </c>
+      <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="5">
         <f>B13*C13/D13</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="B14" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="5">
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
         <f>B14*C14/D14</f>
-        <v>0.05</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B15" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E15" s="5">
         <f>B15*C15/D15</f>
-        <v>0.05</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>39</v>
+      <c r="A16" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B16" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="5">
         <f>B16*C16/D16</f>
-        <v>0.04</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>4</v>
+      <c r="A17" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B17" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="5">
         <f>B17*C17/D17</f>
-        <v>0.04</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E18" s="5">
         <f>B18*C18/D18</f>
-        <v>0.03</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="B19" s="1">
-        <v>0.01</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
         <v>5</v>
       </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-      <c r="E19" s="5">
+      <c r="E19" s="1">
         <f>B19*C19/D19</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1">
         <v>0.01</v>
@@ -942,34 +965,34 @@
         <v>5</v>
       </c>
       <c r="D20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5">
         <f>B20*C20/D20</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1">
         <v>0.01</v>
       </c>
       <c r="C21" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="5">
         <f>B21*C21/D21</f>
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1">
         <v>0.01</v>
@@ -978,34 +1001,34 @@
         <v>4</v>
       </c>
       <c r="D22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="5">
         <f>B22*C22/D22</f>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>40</v>
+      <c r="A23" t="s">
+        <v>4</v>
       </c>
       <c r="B23" s="1">
         <v>0.01</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5">
         <f>B23*C23/D23</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>34</v>
+      <c r="A24" t="s">
+        <v>3</v>
       </c>
       <c r="B24" s="1">
         <v>0.01</v>
@@ -1014,70 +1037,70 @@
         <v>3</v>
       </c>
       <c r="D24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" s="5">
         <f>B24*C24/D24</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" s="1">
         <v>0.01</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
       </c>
       <c r="E25" s="5">
         <f>B25*C25/D25</f>
-        <v>1.4999999999999999E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="B26" s="1">
         <v>0.01</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E26" s="5">
         <f>B26*C26/D26</f>
-        <v>1.3333333333333334E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B27" s="1">
         <v>0.01</v>
       </c>
       <c r="C27" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27" s="5">
         <f>B27*C27/D27</f>
-        <v>1.3333333333333334E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" s="1">
         <v>0.01</v>
@@ -1086,70 +1109,70 @@
         <v>4</v>
       </c>
       <c r="D28" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" s="5">
         <f>B28*C28/D28</f>
-        <v>1.3333333333333334E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>28</v>
+      <c r="A29" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B29" s="1">
         <v>0.01</v>
       </c>
       <c r="C29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E29" s="5">
         <f>B29*C29/D29</f>
-        <v>1.3333333333333334E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>23</v>
+      <c r="A30" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B30" s="1">
         <v>0.01</v>
       </c>
       <c r="C30" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30" s="5">
         <f>B30*C30/D30</f>
-        <v>1.3333333333333334E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B31" s="1">
         <v>0.01</v>
       </c>
       <c r="C31" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" s="5">
         <f>B31*C31/D31</f>
-        <v>1.3333333333333334E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B32" s="1">
         <v>0.01</v>
@@ -1167,7 +1190,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1">
         <v>0.01</v>
@@ -1185,7 +1208,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B34" s="1">
         <v>0.01</v>
@@ -1203,7 +1226,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B35" s="1">
         <v>0.01</v>
@@ -1220,8 +1243,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
-        <v>49</v>
+      <c r="A36" t="s">
+        <v>23</v>
       </c>
       <c r="B36" s="1">
         <v>0.01</v>
@@ -1239,43 +1262,43 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B37" s="1">
         <v>0.01</v>
       </c>
       <c r="C37" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" s="5">
         <f>B37*C37/D37</f>
-        <v>1.2500000000000001E-2</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="B38" s="1">
         <v>0.01</v>
       </c>
       <c r="C38" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E38" s="5">
         <f>B38*C38/D38</f>
-        <v>1.2500000000000001E-2</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B39" s="1">
         <v>0.01</v>
@@ -1284,16 +1307,16 @@
         <v>4</v>
       </c>
       <c r="D39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E39" s="5">
         <f>B39*C39/D39</f>
-        <v>0.01</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B40" s="1">
         <v>0.01</v>
@@ -1302,34 +1325,34 @@
         <v>4</v>
       </c>
       <c r="D40" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40" s="5">
         <f>B40*C40/D40</f>
-        <v>0.01</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>19</v>
+      <c r="A41" t="s">
+        <v>41</v>
       </c>
       <c r="B41" s="1">
         <v>0.01</v>
       </c>
       <c r="C41" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D41" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E41" s="5">
         <f>B41*C41/D41</f>
-        <v>0.01</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>48</v>
+      <c r="A42" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B42" s="1">
         <v>0.01</v>
@@ -1338,124 +1361,250 @@
         <v>4</v>
       </c>
       <c r="D42" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E42" s="5">
         <f>B42*C42/D42</f>
-        <v>8.0000000000000002E-3</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>44</v>
+      <c r="A43" t="s">
+        <v>18</v>
       </c>
       <c r="B43" s="1">
         <v>0.01</v>
       </c>
       <c r="C43" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D43" s="1">
         <v>4</v>
       </c>
       <c r="E43" s="5">
         <f>B43*C43/D43</f>
-        <v>7.4999999999999997E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B44" s="1">
         <v>0.01</v>
       </c>
       <c r="C44" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D44" s="1">
         <v>4</v>
       </c>
       <c r="E44" s="5">
         <f>B44*C44/D44</f>
-        <v>7.4999999999999997E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>21</v>
-      </c>
-      <c r="B45" s="1">
+        <v>10</v>
+      </c>
+      <c r="B45" s="2">
         <v>0.01</v>
       </c>
       <c r="C45" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D45" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E45" s="5">
         <f>B45*C45/D45</f>
-        <v>7.4999999999999997E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B46" s="1">
         <v>0.01</v>
       </c>
       <c r="C46" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D46" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E46" s="5">
         <f>B46*C46/D46</f>
-        <v>6.6666666666666671E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>45</v>
+      <c r="A47" t="s">
+        <v>20</v>
       </c>
       <c r="B47" s="1">
-        <v>-1</v>
+        <v>0.01</v>
       </c>
       <c r="C47" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E47" s="5">
         <f>B47*C47/D47</f>
-        <v>-1.6666666666666667</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>31</v>
+      <c r="A48" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B48" s="1">
-        <v>-1</v>
+        <v>0.01</v>
       </c>
       <c r="C48" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D48" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E48" s="5">
         <f>B48*C48/D48</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C49" s="1">
+        <v>4</v>
+      </c>
+      <c r="D49" s="1">
+        <v>5</v>
+      </c>
+      <c r="E49" s="5">
+        <f>B49*C49/D49</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C50" s="1">
+        <v>3</v>
+      </c>
+      <c r="D50" s="1">
+        <v>4</v>
+      </c>
+      <c r="E50" s="5">
+        <f>B50*C50/D50</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>33</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C51" s="1">
+        <v>3</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4</v>
+      </c>
+      <c r="E51" s="5">
+        <f>B51*C51/D51</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4</v>
+      </c>
+      <c r="E52" s="5">
+        <f>B52*C52/D52</f>
+        <v>7.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="C53" s="1">
+        <v>2</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3</v>
+      </c>
+      <c r="E53" s="5">
+        <f>B53*C53/D53</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>5</v>
+      </c>
+      <c r="D54" s="1">
+        <v>3</v>
+      </c>
+      <c r="E54" s="5">
+        <f>B54*C54/D54</f>
+        <v>-1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C55" s="1">
+        <v>4</v>
+      </c>
+      <c r="D55" s="1">
+        <v>1</v>
+      </c>
+      <c r="E55" s="5">
+        <f>B55*C55/D55</f>
         <v>-4</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E12">
-    <sortState ref="A2:E48">
+    <sortState ref="A2:E55">
       <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>
@@ -1463,311 +1612,311 @@
     <sortCondition descending="1" ref="E2:E11"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D47">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32:C47">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B34">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D36">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C31">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B30">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E47">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C47">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D47">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D47">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C47">
-    <cfRule type="colorScale" priority="53">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
-    <cfRule type="colorScale" priority="24">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="colorScale" priority="22">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="23">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="21">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="colorScale" priority="18">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D36">
-    <cfRule type="colorScale" priority="69">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C31">
-    <cfRule type="colorScale" priority="71">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B30">
-    <cfRule type="colorScale" priority="73">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="74">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E47">
-    <cfRule type="colorScale" priority="77">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C47">
-    <cfRule type="colorScale" priority="79">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D47">
-    <cfRule type="colorScale" priority="81">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
Many small improvements to operation.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -200,9 +200,6 @@
     <t>Save profile</t>
   </si>
   <si>
-    <t>Save points (autoprofile tab)</t>
-  </si>
-  <si>
     <t>Fix autosize columns?</t>
   </si>
   <si>
@@ -213,6 +210,21 @@
   </si>
   <si>
     <t>Autoprofile first cell filename</t>
+  </si>
+  <si>
+    <t>No resume until waiting</t>
+  </si>
+  <si>
+    <t>Time/Assured on screen</t>
+  </si>
+  <si>
+    <t>Move to point N</t>
+  </si>
+  <si>
+    <t>Save points</t>
+  </si>
+  <si>
+    <t>"New Set" cancel</t>
   </si>
 </sst>
 </file>
@@ -598,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +622,7 @@
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -626,13 +638,13 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -643,50 +655,50 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="5">
         <f>B2*C2/D2</f>
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="5">
         <f>B3*C3/D3</f>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>56</v>
+      <c r="A4" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
         <f>B4*C4/D4</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
+      <c r="A5" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -695,124 +707,124 @@
         <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
         <f>B5*C5/D5</f>
-        <v>3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="1">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="5">
         <f>B6*C6/D6</f>
-        <v>2</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>35</v>
+      <c r="A7" t="s">
+        <v>46</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="5">
         <f>B7*C7/D7</f>
-        <v>1.5</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>54</v>
+      <c r="A8" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="5">
         <f>B8*C8/D8</f>
-        <v>1.5</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="5">
         <f>B9*C9/D9</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="5">
         <f>B10*C10/D10</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>51</v>
+      <c r="A11" t="s">
+        <v>53</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="5">
         <f>B11*C11/D11</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -821,142 +833,142 @@
         <v>3</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E12" s="5">
         <f>B12*C12/D12</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>43</v>
+      <c r="A13" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="5">
         <f>B13*C13/D13</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>53</v>
+      <c r="A14" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="5">
         <f>B14*C14/D14</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5">
         <f>B15*C15/D15</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>29</v>
+      <c r="A16" t="s">
+        <v>54</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16" s="5">
         <f>B16*C16/D16</f>
-        <v>0.66666666666666663</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>30</v>
+      <c r="A17" t="s">
+        <v>62</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" s="5">
         <f>B17*C17/D17</f>
-        <v>0.66666666666666663</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E18" s="5">
         <f>B18*C18/D18</f>
-        <v>0.66666666666666663</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1">
-        <v>1</v>
+        <v>0.01</v>
       </c>
       <c r="C19" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1">
-        <v>5</v>
-      </c>
-      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="5">
         <f>B19*C19/D19</f>
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1">
         <v>0.01</v>
@@ -974,7 +986,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1">
         <v>0.01</v>
@@ -1028,7 +1040,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1">
         <v>0.01</v>
@@ -1046,25 +1058,25 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B25" s="1">
         <v>0.01</v>
       </c>
       <c r="C25" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" s="5">
         <f>B25*C25/D25</f>
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1">
         <v>0.01</v>
@@ -1082,34 +1094,34 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B27" s="1">
         <v>0.01</v>
       </c>
       <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="1">
         <v>2</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
       </c>
       <c r="E27" s="5">
         <f>B27*C27/D27</f>
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B28" s="1">
         <v>0.01</v>
       </c>
       <c r="C28" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="5">
         <f>B28*C28/D28</f>
@@ -1117,26 +1129,26 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>40</v>
+      <c r="A29" t="s">
+        <v>24</v>
       </c>
       <c r="B29" s="1">
         <v>0.01</v>
       </c>
       <c r="C29" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1">
         <v>2</v>
       </c>
       <c r="E29" s="5">
         <f>B29*C29/D29</f>
-        <v>1.4999999999999999E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>34</v>
+      <c r="A30" t="s">
+        <v>61</v>
       </c>
       <c r="B30" s="1">
         <v>0.01</v>
@@ -1153,8 +1165,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>17</v>
+      <c r="A31" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>0.01</v>
@@ -1171,44 +1183,44 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>32</v>
+      <c r="A32" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B32" s="1">
         <v>0.01</v>
       </c>
       <c r="C32" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E32" s="5">
         <f>B32*C32/D32</f>
-        <v>1.3333333333333334E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B33" s="1">
         <v>0.01</v>
       </c>
       <c r="C33" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E33" s="5">
         <f>B33*C33/D33</f>
-        <v>1.3333333333333334E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1">
         <v>0.01</v>
@@ -1226,7 +1238,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="1">
         <v>0.01</v>
@@ -1244,7 +1256,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1">
         <v>0.01</v>
@@ -1262,7 +1274,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B37" s="1">
         <v>0.01</v>
@@ -1280,7 +1292,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B38" s="1">
         <v>0.01</v>
@@ -1298,7 +1310,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B39" s="1">
         <v>0.01</v>
@@ -1316,7 +1328,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B40" s="1">
         <v>0.01</v>
@@ -1334,7 +1346,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B41" s="1">
         <v>0.01</v>
@@ -1351,8 +1363,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>49</v>
+      <c r="A42" t="s">
+        <v>12</v>
       </c>
       <c r="B42" s="1">
         <v>0.01</v>
@@ -1370,88 +1382,88 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1">
         <v>0.01</v>
       </c>
       <c r="C43" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D43" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43" s="5">
         <f>B43*C43/D43</f>
-        <v>1.2500000000000001E-2</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>1</v>
+      <c r="A44" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B44" s="1">
         <v>0.01</v>
       </c>
       <c r="C44" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D44" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E44" s="5">
         <f>B44*C44/D44</f>
-        <v>1.2500000000000001E-2</v>
+        <v>1.3333333333333334E-2</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" s="2">
+        <v>18</v>
+      </c>
+      <c r="B45" s="1">
         <v>0.01</v>
       </c>
       <c r="C45" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D45" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E45" s="5">
         <f>B45*C45/D45</f>
-        <v>0.01</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B46" s="1">
         <v>0.01</v>
       </c>
       <c r="C46" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46" s="1">
         <v>4</v>
       </c>
       <c r="E46" s="5">
         <f>B46*C46/D46</f>
-        <v>0.01</v>
+        <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>20</v>
-      </c>
-      <c r="B47" s="1">
+        <v>10</v>
+      </c>
+      <c r="B47" s="2">
         <v>0.01</v>
       </c>
       <c r="C47" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E47" s="5">
         <f>B47*C47/D47</f>
@@ -1459,17 +1471,17 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
-        <v>19</v>
+      <c r="A48" t="s">
+        <v>13</v>
       </c>
       <c r="B48" s="1">
         <v>0.01</v>
       </c>
       <c r="C48" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E48" s="5">
         <f>B48*C48/D48</f>
@@ -1478,7 +1490,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B49" s="1">
         <v>0.01</v>
@@ -1487,52 +1499,52 @@
         <v>4</v>
       </c>
       <c r="D49" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" s="5">
         <f>B49*C49/D49</f>
-        <v>8.0000000000000002E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="B50" s="1">
         <v>0.01</v>
       </c>
       <c r="C50" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D50" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E50" s="5">
         <f>B50*C50/D50</f>
-        <v>7.4999999999999997E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B51" s="1">
         <v>0.01</v>
       </c>
       <c r="C51" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D51" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E51" s="5">
         <f>B51*C51/D51</f>
-        <v>7.4999999999999997E-3</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>21</v>
+      <c r="A52" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B52" s="1">
         <v>0.01</v>
@@ -1550,61 +1562,133 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B53" s="1">
         <v>0.01</v>
       </c>
       <c r="C53" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D53" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E53" s="5">
         <f>B53*C53/D53</f>
-        <v>6.6666666666666671E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>45</v>
+      <c r="A54" t="s">
+        <v>21</v>
       </c>
       <c r="B54" s="1">
-        <v>-1</v>
+        <v>0.01</v>
       </c>
       <c r="C54" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D54" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E54" s="5">
         <f>B54*C54/D54</f>
-        <v>-1.6666666666666667</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>31</v>
+      <c r="A55" t="s">
+        <v>50</v>
       </c>
       <c r="B55" s="1">
-        <v>-1</v>
+        <v>0.01</v>
       </c>
       <c r="C55" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D55" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E55" s="5">
         <f>B55*C55/D55</f>
+        <v>6.6666666666666671E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B56" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C56" s="1">
+        <v>5</v>
+      </c>
+      <c r="D56" s="1">
+        <v>3</v>
+      </c>
+      <c r="E56" s="5">
+        <f>B56*C56/D56</f>
+        <v>-1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>4</v>
+      </c>
+      <c r="D57" s="1">
+        <v>2</v>
+      </c>
+      <c r="E57" s="5">
+        <f>B57*C57/D57</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C58" s="1">
+        <v>3</v>
+      </c>
+      <c r="D58" s="1">
+        <v>1</v>
+      </c>
+      <c r="E58" s="5">
+        <f>B58*C58/D58</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1</v>
+      </c>
+      <c r="E59" s="5">
+        <f>B59*C59/D59</f>
         <v>-4</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E12">
-    <sortState ref="A2:E55">
+    <sortState ref="A2:E59">
       <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Autoprofiles now require the filename as the first line.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A7D2E1-9FCB-4304-9E8A-F08121A8ACD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F802DD68-D054-412F-8C41-8016FAEC2403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{74984FB7-307A-4321-AFAB-CFDB5763E27F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Produce sensor file</t>
   </si>
   <si>
-    <t>Load a sensor file?</t>
-  </si>
-  <si>
     <t>Put transform on display</t>
   </si>
   <si>
@@ -162,12 +159,6 @@
     <t>Details draw from job</t>
   </si>
   <si>
-    <t>Floating graphs/kill graphs</t>
-  </si>
-  <si>
-    <t>Fix datafile filenames?</t>
-  </si>
-  <si>
     <t>Job names</t>
   </si>
   <si>
@@ -187,6 +178,63 @@
   </si>
   <si>
     <t>Freeze if point moves during scroll</t>
+  </si>
+  <si>
+    <t>Autoprofile actions</t>
+  </si>
+  <si>
+    <t>Kill graphs</t>
+  </si>
+  <si>
+    <t>Detract graphs</t>
+  </si>
+  <si>
+    <t>Fix datafile filenames</t>
+  </si>
+  <si>
+    <t>Julabo FP79</t>
+  </si>
+  <si>
+    <t>Cancel load profile</t>
+  </si>
+  <si>
+    <t>Save profile</t>
+  </si>
+  <si>
+    <t>Fix autosize columns?</t>
+  </si>
+  <si>
+    <t>Restart point</t>
+  </si>
+  <si>
+    <t>Reset autoprofile</t>
+  </si>
+  <si>
+    <t>Autoprofile first cell filename</t>
+  </si>
+  <si>
+    <t>No resume until waiting</t>
+  </si>
+  <si>
+    <t>Time/Assured on screen</t>
+  </si>
+  <si>
+    <t>Move to point N</t>
+  </si>
+  <si>
+    <t>Save points</t>
+  </si>
+  <si>
+    <t>"New Set" cancel</t>
+  </si>
+  <si>
+    <t>Fix key errors in old jobs and instruments</t>
+  </si>
+  <si>
+    <t>Fix graph saving?</t>
+  </si>
+  <si>
+    <t>Clear comment box after points are recorded</t>
   </si>
 </sst>
 </file>
@@ -196,7 +244,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,16 +254,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -238,7 +292,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -248,7 +302,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,20 +619,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0875FA9E-03C5-44EF-91A8-26A2DEEA24CC}">
-  <dimension ref="A1:E46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -585,829 +642,1117 @@
       <c r="B1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>32</v>
+      <c r="A2" t="s">
+        <v>56</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <f t="shared" ref="E2:E46" si="0">B2*C2/D2</f>
-        <v>4</v>
+        <f>B2*C2/D2</f>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>45</v>
+      <c r="A3" t="s">
+        <v>63</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>B3*C3/D3</f>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="C4" s="1">
+        <v>4</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6666666666666667</v>
+        <f>B4*C4/D4</f>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
         <v>2</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="0"/>
+        <f>B5*C5/D5</f>
         <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-      <c r="D6">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1">
         <v>3</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="0"/>
+        <f>B6*C6/D6</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>49</v>
+      <c r="A7" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
+      <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
+        <f>B7*C7/D7</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>3</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="0"/>
+        <f>B8*C8/D8</f>
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="0"/>
+        <f>B9*C9/D9</f>
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
+      <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>B10*C10/D10</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>41</v>
+      <c r="A11" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
-      <c r="C11">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
+        <f>B11*C11/D11</f>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>2</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>3</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="0"/>
+        <f>B12*C12/D12</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="0"/>
+        <f>B13*C13/D13</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>3</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="0"/>
+        <f>B14*C14/D14</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>4</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="0"/>
+        <f>B15*C15/D15</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>3</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>5</v>
       </c>
       <c r="E16" s="5">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <f>B16*C16/D16</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="E17" s="5">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <f>B17*C17/D17</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="B18" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
         <v>5</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>1</v>
       </c>
       <c r="E18" s="5">
-        <f t="shared" si="0"/>
-        <v>0.05</v>
+        <f>B18*C18/D18</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C19">
-        <v>4</v>
-      </c>
-      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="E19" s="5">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>B19*C19/D19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B20" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5</v>
+      </c>
+      <c r="D20" s="1">
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <f t="shared" si="0"/>
-        <v>0.04</v>
+        <f>B20*C20/D20</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B21" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
         <v>1</v>
       </c>
       <c r="E21" s="5">
-        <f t="shared" si="0"/>
-        <v>0.03</v>
+        <f>B21*C21/D21</f>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C22">
-        <v>5</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <f>B22*C22/D22</f>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C23">
-        <v>5</v>
-      </c>
-      <c r="D23">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1</v>
       </c>
       <c r="E23" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5000000000000001E-2</v>
+        <f>B23*C23/D23</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+      <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="E24" s="5">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
+        <f>B24*C24/D24</f>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B25" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="5">
+        <f>B25*C25/D25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
         <v>2</v>
       </c>
-      <c r="E25" s="5">
-        <f t="shared" si="0"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B26" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C26">
-        <v>3</v>
-      </c>
-      <c r="D26">
-        <v>2</v>
+      <c r="D26" s="1">
+        <v>1</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
+        <f>B26*C26/D26</f>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>2</v>
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
+        <f>B27*C27/D27</f>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C28">
-        <v>3</v>
-      </c>
-      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1">
         <v>2</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4999999999999999E-2</v>
+        <f>B28*C28/D28</f>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="B29" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>5</v>
+      </c>
+      <c r="D29" s="1">
+        <v>2</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B29*C29/D29</f>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B30" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C30">
-        <v>4</v>
-      </c>
-      <c r="D30">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>4</v>
+      </c>
+      <c r="D30" s="1">
+        <v>2</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B30*C30/D30</f>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B31" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C31">
-        <v>4</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B31*C31/D31</f>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>29</v>
+      <c r="A32" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B32" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C32">
-        <v>4</v>
-      </c>
-      <c r="D32">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B32*C32/D32</f>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>24</v>
+      <c r="A33" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B33" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-      <c r="D33">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>2</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B33*C33/D33</f>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B34" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C34">
-        <v>4</v>
-      </c>
-      <c r="D34">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1">
+        <v>2</v>
       </c>
       <c r="E34" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B34*C34/D34</f>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B35" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
         <v>3</v>
       </c>
       <c r="E35" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B35*C35/D35</f>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
         <v>3</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B36*C36/D36</f>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B37" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C37">
-        <v>4</v>
-      </c>
-      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>4</v>
+      </c>
+      <c r="D37" s="1">
         <v>3</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B37*C37/D37</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>4</v>
+      </c>
+      <c r="D38" s="1">
         <v>3</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3333333333333334E-2</v>
+        <f>B38*C38/D38</f>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B39" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C39">
-        <v>5</v>
-      </c>
-      <c r="D39">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>4</v>
+      </c>
+      <c r="D39" s="1">
+        <v>3</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2500000000000001E-2</v>
+        <f>B39*C39/D39</f>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B40" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C40">
-        <v>5</v>
-      </c>
-      <c r="D40">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C40" s="1">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1">
+        <v>3</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2500000000000001E-2</v>
+        <f>B40*C40/D40</f>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B41" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C41">
-        <v>4</v>
-      </c>
-      <c r="D41">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>4</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
+        <f>B41*C41/D41</f>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B42" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
-      <c r="D42">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C42" s="1">
+        <v>4</v>
+      </c>
+      <c r="D42" s="1">
+        <v>3</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
+        <f>B42*C42/D42</f>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
-        <v>47</v>
+      <c r="A43" t="s">
+        <v>12</v>
       </c>
       <c r="B43" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-      <c r="D43">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1">
+        <v>3</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
+        <f>B43*C43/D43</f>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B44" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C44">
-        <v>3</v>
-      </c>
-      <c r="D44">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C44" s="1">
+        <v>4</v>
+      </c>
+      <c r="D44" s="1">
+        <v>3</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
+        <f>B44*C44/D44</f>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>22</v>
+      <c r="A45" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B45" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C45">
-        <v>3</v>
-      </c>
-      <c r="D45">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>4</v>
+      </c>
+      <c r="D45" s="1">
+        <v>3</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="0"/>
-        <v>7.4999999999999997E-3</v>
+        <f>B45*C45/D45</f>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B46" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <v>3</v>
+      </c>
+      <c r="D46" s="1">
+        <v>3</v>
+      </c>
+      <c r="E46" s="5">
+        <f>B46*C46/D46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0</v>
+      </c>
+      <c r="C47" s="1">
         <v>2</v>
       </c>
-      <c r="D46">
-        <v>3</v>
-      </c>
-      <c r="E46" s="5">
-        <f t="shared" si="0"/>
-        <v>6.6666666666666671E-3</v>
+      <c r="D47" s="1">
+        <v>3</v>
+      </c>
+      <c r="E47" s="5">
+        <f>B47*C47/D47</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>18</v>
+      </c>
+      <c r="B48" s="1">
+        <v>0</v>
+      </c>
+      <c r="C48" s="1">
+        <v>5</v>
+      </c>
+      <c r="D48" s="1">
+        <v>4</v>
+      </c>
+      <c r="E48" s="5">
+        <f>B48*C48/D48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="1">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1">
+        <v>5</v>
+      </c>
+      <c r="D49" s="1">
+        <v>4</v>
+      </c>
+      <c r="E49" s="5">
+        <f>B49*C49/D49</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="1">
+        <v>0</v>
+      </c>
+      <c r="C50" s="1">
+        <v>4</v>
+      </c>
+      <c r="D50" s="1">
+        <v>4</v>
+      </c>
+      <c r="E50" s="5">
+        <f>B50*C50/D50</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="1">
+        <v>0</v>
+      </c>
+      <c r="C51" s="1">
+        <v>4</v>
+      </c>
+      <c r="D51" s="1">
+        <v>4</v>
+      </c>
+      <c r="E51" s="5">
+        <f>B51*C51/D51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B52" s="1">
+        <v>0</v>
+      </c>
+      <c r="C52" s="1">
+        <v>3</v>
+      </c>
+      <c r="D52" s="1">
+        <v>4</v>
+      </c>
+      <c r="E52" s="5">
+        <f>B52*C52/D52</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>33</v>
+      </c>
+      <c r="B53" s="1">
+        <v>0</v>
+      </c>
+      <c r="C53" s="1">
+        <v>3</v>
+      </c>
+      <c r="D53" s="1">
+        <v>4</v>
+      </c>
+      <c r="E53" s="5">
+        <f>B53*C53/D53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="1">
+        <v>0</v>
+      </c>
+      <c r="C54" s="1">
+        <v>3</v>
+      </c>
+      <c r="D54" s="1">
+        <v>4</v>
+      </c>
+      <c r="E54" s="5">
+        <f>B54*C54/D54</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="1">
+        <v>0</v>
+      </c>
+      <c r="C55" s="1">
+        <v>5</v>
+      </c>
+      <c r="D55" s="1">
+        <v>5</v>
+      </c>
+      <c r="E55" s="5">
+        <f>B55*C55/D55</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>48</v>
+      </c>
+      <c r="B56" s="1">
+        <v>0</v>
+      </c>
+      <c r="C56" s="1">
+        <v>4</v>
+      </c>
+      <c r="D56" s="1">
+        <v>5</v>
+      </c>
+      <c r="E56" s="5">
+        <f>B56*C56/D56</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B57" s="2">
+        <v>-1</v>
+      </c>
+      <c r="C57" s="1">
+        <v>4</v>
+      </c>
+      <c r="D57" s="1">
+        <v>3</v>
+      </c>
+      <c r="E57" s="5">
+        <f>B57*C57/D57</f>
+        <v>-1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C58" s="1">
+        <v>5</v>
+      </c>
+      <c r="D58" s="1">
+        <v>3</v>
+      </c>
+      <c r="E58" s="5">
+        <f>B58*C58/D58</f>
+        <v>-1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>4</v>
+      </c>
+      <c r="D59" s="1">
+        <v>2</v>
+      </c>
+      <c r="E59" s="5">
+        <f>B59*C59/D59</f>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C60" s="1">
+        <v>3</v>
+      </c>
+      <c r="D60" s="1">
+        <v>1</v>
+      </c>
+      <c r="E60" s="5">
+        <f>B60*C60/D60</f>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>57</v>
+      </c>
+      <c r="B61" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C61" s="1">
+        <v>4</v>
+      </c>
+      <c r="D61" s="1">
+        <v>1</v>
+      </c>
+      <c r="E61" s="5">
+        <f>B61*C61/D61</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C62" s="1">
+        <v>4</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1</v>
+      </c>
+      <c r="E62" s="5">
+        <f>B62*C62/D62</f>
+        <v>-4</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E12" xr:uid="{B709D02C-7123-424C-8570-C29FC5B5BAA2}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E46">
+  <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E62">
       <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>
@@ -1426,8 +1771,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:D46">
-    <cfRule type="colorScale" priority="47">
+  <conditionalFormatting sqref="D35:D47">
+    <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1436,8 +1781,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33:C46">
-    <cfRule type="colorScale" priority="49">
+  <conditionalFormatting sqref="C32:C47">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1447,7 +1812,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1457,7 +1822,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1467,7 +1832,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1477,7 +1842,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1487,7 +1852,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1497,7 +1862,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1507,7 +1872,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1517,7 +1882,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1527,7 +1892,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1537,7 +1902,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1547,7 +1912,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1557,7 +1922,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1567,7 +1932,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1577,7 +1942,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1587,7 +1952,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1597,7 +1962,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -1606,93 +1971,105 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
+  <conditionalFormatting sqref="D2:D36">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C31">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B30">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="76">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E47">
+    <cfRule type="colorScale" priority="79">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C47">
+    <cfRule type="colorScale" priority="81">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D47">
+    <cfRule type="colorScale" priority="83">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E1:E1048576">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D37">
-    <cfRule type="colorScale" priority="50">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C32">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B31">
-    <cfRule type="colorScale" priority="57">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="58">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E46">
-    <cfRule type="colorScale" priority="61">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C46">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D46">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FFF8696B"/>
       </colorScale>

</xml_diff>

<commit_message>
Autoprofile now can perform actions, has a "no change" option, and sets the setpoints on loading.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F802DD68-D054-412F-8C41-8016FAEC2403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95F29EB-9C9A-4138-82E8-1F2776CFD8A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Freeze if point moves during scroll</t>
   </si>
   <si>
-    <t>Autoprofile actions</t>
-  </si>
-  <si>
     <t>Kill graphs</t>
   </si>
   <si>
@@ -235,6 +232,12 @@
   </si>
   <si>
     <t>Clear comment box after points are recorded</t>
+  </si>
+  <si>
+    <t>Autoprofile actions/actionwrite lists</t>
+  </si>
+  <si>
+    <t>- means "don't write"</t>
   </si>
 </sst>
 </file>
@@ -292,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +309,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -653,98 +657,98 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>56</v>
+      <c r="A2" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="5">
         <f>B2*C2/D2</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="5">
         <f>B3*C3/D3</f>
-        <v>3</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
-        <v>42</v>
+      <c r="A4" t="s">
+        <v>62</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
       </c>
       <c r="E4" s="5">
         <f>B4*C4/D4</f>
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
-        <v>35</v>
+      <c r="A5" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="5">
         <f>B5*C5/D5</f>
-        <v>1.5</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
       </c>
       <c r="E6" s="5">
         <f>B6*C6/D6</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>51</v>
+      <c r="A7" t="s">
+        <v>63</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -753,70 +757,70 @@
         <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E7" s="5">
         <f>B7*C7/D7</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>43</v>
+      <c r="A8" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="5">
         <f>B8*C8/D8</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>53</v>
+      <c r="A9" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="5">
         <f>B9*C9/D9</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E10" s="5">
         <f>B10*C10/D10</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>29</v>
+      <c r="A11" t="s">
+        <v>64</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -833,98 +837,98 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>30</v>
+      <c r="A12" t="s">
+        <v>53</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12" s="5">
         <f>B12*C12/D12</f>
-        <v>0.66666666666666663</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13" s="5">
         <f>B13*C13/D13</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" s="5">
         <f>B14*C14/D14</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5">
         <f>B15*C15/D15</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E16" s="5">
         <f>B16*C16/D16</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -942,13 +946,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
       </c>
       <c r="C18" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -960,13 +964,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -978,13 +982,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -995,14 +999,14 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>52</v>
+      <c r="A21" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
       <c r="C21" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1014,13 +1018,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1032,13 +1036,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
       <c r="C23" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -1050,7 +1054,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1068,7 +1072,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1157,7 +1161,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B30" s="1">
@@ -1176,13 +1180,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1">
         <v>2</v>
@@ -1193,8 +1197,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
-        <v>40</v>
+      <c r="A32" t="s">
+        <v>60</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1212,7 +1216,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -1229,8 +1233,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>17</v>
+      <c r="A34" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -1248,16 +1252,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E35" s="5">
         <f>B35*C35/D35</f>
@@ -1265,14 +1269,14 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>27</v>
+      <c r="A36" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
       </c>
       <c r="C36" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D36" s="1">
         <v>3</v>
@@ -1283,8 +1287,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>26</v>
+      <c r="A37" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -1301,8 +1305,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>28</v>
+      <c r="A38" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -1319,8 +1323,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>23</v>
+      <c r="A39" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -1337,8 +1341,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>25</v>
+      <c r="A40" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
@@ -1355,8 +1359,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>22</v>
+      <c r="A41" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -1373,8 +1377,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>9</v>
+      <c r="A42" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -1392,7 +1396,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -1410,7 +1414,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -1427,8 +1431,8 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="4" t="s">
-        <v>49</v>
+      <c r="A45" t="s">
+        <v>12</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -1446,13 +1450,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D46" s="1">
         <v>3</v>
@@ -1463,14 +1467,14 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>50</v>
+      <c r="A47" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
       </c>
       <c r="C47" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D47" s="1">
         <v>3</v>
@@ -1481,17 +1485,17 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>18</v>
-      </c>
-      <c r="B48" s="1">
+      <c r="A48" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="2">
         <v>0</v>
       </c>
       <c r="C48" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D48" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48" s="5">
         <f>B48*C48/D48</f>
@@ -1500,16 +1504,16 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
       </c>
       <c r="C49" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D49" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E49" s="5">
         <f>B49*C49/D49</f>
@@ -1518,16 +1522,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
       </c>
       <c r="C50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E50" s="5">
         <f>B50*C50/D50</f>
@@ -1536,16 +1540,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
       </c>
       <c r="C51" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D51" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E51" s="5">
         <f>B51*C51/D51</f>
@@ -1553,14 +1557,14 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
-        <v>44</v>
+      <c r="A52" t="s">
+        <v>18</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
       </c>
       <c r="C52" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D52" s="1">
         <v>4</v>
@@ -1572,13 +1576,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
       </c>
       <c r="C53" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D53" s="1">
         <v>4</v>
@@ -1589,14 +1593,14 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>21</v>
+      <c r="A54" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
       </c>
       <c r="C54" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D54" s="1">
         <v>4</v>
@@ -1607,17 +1611,17 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
-        <v>19</v>
+      <c r="A55" t="s">
+        <v>20</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
       </c>
       <c r="C55" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E55" s="5">
         <f>B55*C55/D55</f>
@@ -1625,17 +1629,17 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>48</v>
+      <c r="A56" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D56" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E56" s="5">
         <f>B56*C56/D56</f>
@@ -1643,116 +1647,134 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B57" s="2">
-        <v>-1</v>
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57" s="1">
+        <v>0</v>
       </c>
       <c r="C57" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E57" s="5">
         <f>B57*C57/D57</f>
-        <v>-1.3333333333333333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="3" t="s">
-        <v>45</v>
+      <c r="A58" t="s">
+        <v>21</v>
       </c>
       <c r="B58" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D58" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E58" s="5">
         <f>B58*C58/D58</f>
-        <v>-1.6666666666666667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>59</v>
+      <c r="A59" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B59" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D59" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E59" s="5">
         <f>B59*C59/D59</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B60" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C60" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D60" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E60" s="5">
         <f>B60*C60/D60</f>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="B61" s="1">
         <v>-1</v>
       </c>
       <c r="C61" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E61" s="5">
         <f>B61*C61/D61</f>
-        <v>-4</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="3" t="s">
-        <v>31</v>
+      <c r="A62" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="B62" s="1">
         <v>-1</v>
       </c>
       <c r="C62" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E62" s="5">
         <f>B62*C62/D62</f>
-        <v>-4</v>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C63" s="1">
+        <v>3</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2</v>
+      </c>
+      <c r="E63" s="5">
+        <f>B63*C63/D63</f>
+        <v>-1.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E62">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E63">
       <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
"Writing" printed on screen
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95F29EB-9C9A-4138-82E8-1F2776CFD8A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635C5073-57B2-4E55-A9CD-C23CEA264A71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>- means "don't write"</t>
+  </si>
+  <si>
+    <t>"Writing" on screen</t>
   </si>
 </sst>
 </file>
@@ -624,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,43 +823,43 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E11" s="5">
         <f>B11*C11/D11</f>
-        <v>0.66666666666666663</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E12" s="5">
         <f>B12*C12/D12</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -874,7 +877,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -892,7 +895,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -910,7 +913,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -928,13 +931,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -1540,7 +1543,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -1558,16 +1561,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
       </c>
       <c r="C52" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D52" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E52" s="5">
         <f>B52*C52/D52</f>
@@ -1576,7 +1579,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1593,14 +1596,14 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="3" t="s">
-        <v>13</v>
+      <c r="A54" t="s">
+        <v>1</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
       </c>
       <c r="C54" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D54" s="1">
         <v>4</v>
@@ -1611,8 +1614,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>20</v>
+      <c r="A55" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -1629,14 +1632,14 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="4" t="s">
-        <v>44</v>
+      <c r="A56" t="s">
+        <v>20</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D56" s="1">
         <v>4</v>
@@ -1647,8 +1650,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>33</v>
+      <c r="A57" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
@@ -1666,7 +1669,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
@@ -1683,17 +1686,17 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
-        <v>19</v>
+      <c r="A59" t="s">
+        <v>21</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D59" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E59" s="5">
         <f>B59*C59/D59</f>
@@ -1701,14 +1704,14 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>47</v>
+      <c r="A60" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="C60" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D60" s="1">
         <v>5</v>
@@ -1720,25 +1723,25 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="B61" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C61" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D61" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E61" s="5">
         <f>B61*C61/D61</f>
-        <v>-0.75</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="7" t="s">
-        <v>66</v>
+      <c r="A62" t="s">
+        <v>65</v>
       </c>
       <c r="B62" s="1">
         <v>-1</v>
@@ -1747,16 +1750,16 @@
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E62" s="5">
         <f>B62*C62/D62</f>
-        <v>-1</v>
+        <v>-0.75</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
-        <v>35</v>
+      <c r="A63" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="B63" s="1">
         <v>-1</v>
@@ -1765,16 +1768,34 @@
         <v>3</v>
       </c>
       <c r="D63" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E63" s="5">
         <f>B63*C63/D63</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B64" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C64" s="1">
+        <v>3</v>
+      </c>
+      <c r="D64" s="1">
+        <v>2</v>
+      </c>
+      <c r="E64" s="5">
+        <f>B64*C64/D64</f>
         <v>-1.5</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E63">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
       <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
TS2500 now has checks and a write_action operation.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4D60AC-0BFE-48A6-9924-06AC518A62CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32745C82-6CBD-4A08-9855-6C63C35831FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -247,6 +247,30 @@
   </si>
   <si>
     <t>Rotation stage</t>
+  </si>
+  <si>
+    <t>mK and uK self-heating checks</t>
+  </si>
+  <si>
+    <t>Uncertainty in instrument files</t>
+  </si>
+  <si>
+    <t>README.md</t>
+  </si>
+  <si>
+    <t>Validate software</t>
+  </si>
+  <si>
+    <t>2900 fan speed?</t>
+  </si>
+  <si>
+    <t>Remind if instrument calibration due</t>
+  </si>
+  <si>
+    <t>Version number</t>
+  </si>
+  <si>
+    <t>Document tracability</t>
   </si>
 </sst>
 </file>
@@ -630,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -664,7 +688,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -673,34 +697,34 @@
         <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
         <f>B2*C2/D2</f>
-        <v>1.6666666666666667</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4">
         <f>B3*C3/D3</f>
-        <v>1.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -709,34 +733,34 @@
         <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4">
         <f>B4*C4/D4</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>49</v>
+      <c r="A5" t="s">
+        <v>72</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="4">
         <f>B5*C5/D5</f>
-        <v>1.3333333333333333</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -745,274 +769,274 @@
         <v>4</v>
       </c>
       <c r="D6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" s="4">
         <f>B6*C6/D6</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
         <f>B7*C7/D7</f>
-        <v>0.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
+      <c r="A8" t="s">
+        <v>45</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="4">
         <f>B8*C8/D8</f>
-        <v>0.66666666666666663</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
+      <c r="A9" t="s">
+        <v>60</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
         <v>2</v>
-      </c>
-      <c r="D9" s="1">
-        <v>3</v>
       </c>
       <c r="E9" s="4">
         <f>B9*C9/D9</f>
-        <v>0.66666666666666663</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1">
         <v>2</v>
-      </c>
-      <c r="D10" s="1">
-        <v>3</v>
       </c>
       <c r="E10" s="4">
         <f>B10*C10/D10</f>
-        <v>0.66666666666666663</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="C11" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="4">
         <f>B11*C11/D11</f>
-        <v>0.5</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E12" s="4">
         <f>B12*C12/D12</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E13" s="4">
         <f>B13*C13/D13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4">
         <f>B14*C14/D14</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>36</v>
+      <c r="A15" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E15" s="4">
         <f>B15*C15/D15</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>37</v>
+      <c r="A16" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E16" s="4">
         <f>B16*C16/D16</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="4">
         <f>B17*C17/D17</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>64</v>
+      <c r="A18" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E18" s="4">
         <f>B18*C18/D18</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E19" s="4">
         <f>B19*C19/D19</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E20" s="4">
         <f>B20*C20/D20</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
       </c>
       <c r="C21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1">
         <v>1</v>
@@ -1023,14 +1047,14 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>30</v>
+      <c r="A22" t="s">
+        <v>57</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1042,13 +1066,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
       <c r="C23" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -1060,13 +1084,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -1078,13 +1102,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1096,13 +1120,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1114,16 +1138,16 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="4">
         <f>B27*C27/D27</f>
@@ -1132,16 +1156,16 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
       <c r="C28" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="4">
         <f>B28*C28/D28</f>
@@ -1150,13 +1174,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1168,7 +1192,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1177,7 +1201,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="4">
         <f>B30*C30/D30</f>
@@ -1186,16 +1210,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="4">
         <f>B31*C31/D31</f>
@@ -1203,17 +1227,17 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>44</v>
+      <c r="A32" t="s">
+        <v>52</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
       </c>
       <c r="C32" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D32" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E32" s="4">
         <f>B32*C32/D32</f>
@@ -1222,7 +1246,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -1231,7 +1255,7 @@
         <v>3</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="4">
         <f>B33*C33/D33</f>
@@ -1239,8 +1263,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
-        <v>39</v>
+      <c r="A34" t="s">
+        <v>55</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -1249,7 +1273,7 @@
         <v>3</v>
       </c>
       <c r="D34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="4">
         <f>B34*C34/D34</f>
@@ -1257,14 +1281,14 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
-        <v>33</v>
+      <c r="A35" t="s">
+        <v>15</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
@@ -1276,13 +1300,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
       </c>
       <c r="C36" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D36" s="1">
         <v>2</v>
@@ -1293,17 +1317,17 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
-        <v>34</v>
+      <c r="A37" t="s">
+        <v>10</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
       </c>
       <c r="C37" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="4">
         <f>B37*C37/D37</f>
@@ -1312,7 +1336,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -1321,7 +1345,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" s="4">
         <f>B38*C38/D38</f>
@@ -1329,8 +1353,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
-        <v>26</v>
+      <c r="A39" t="s">
+        <v>56</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -1339,7 +1363,7 @@
         <v>4</v>
       </c>
       <c r="D39" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="4">
         <f>B39*C39/D39</f>
@@ -1347,14 +1371,14 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
-        <v>25</v>
+      <c r="A40" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
       </c>
       <c r="C40" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D40" s="1">
         <v>3</v>
@@ -1365,17 +1389,17 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
-        <v>27</v>
+      <c r="A41" t="s">
+        <v>58</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
       </c>
       <c r="C41" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="4">
         <f>B41*C41/D41</f>
@@ -1383,17 +1407,17 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>22</v>
+      <c r="A42" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
       </c>
       <c r="C42" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42" s="4">
         <f>B42*C42/D42</f>
@@ -1401,17 +1425,17 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>24</v>
+      <c r="A43" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
       </c>
       <c r="C43" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" s="4">
         <f>B43*C43/D43</f>
@@ -1420,16 +1444,16 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
       </c>
       <c r="C44" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" s="4">
         <f>B44*C44/D44</f>
@@ -1437,17 +1461,17 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>8</v>
+      <c r="A45" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
       </c>
       <c r="C45" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E45" s="4">
         <f>B45*C45/D45</f>
@@ -1455,8 +1479,8 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>11</v>
+      <c r="A46" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
@@ -1473,8 +1497,8 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>40</v>
+      <c r="A47" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -1491,8 +1515,8 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="3" t="s">
-        <v>47</v>
+      <c r="A48" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -1509,8 +1533,8 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
-        <v>13</v>
+      <c r="A49" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1527,17 +1551,17 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>17</v>
+      <c r="A50" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
       </c>
       <c r="C50" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E50" s="4">
         <f>B50*C50/D50</f>
@@ -1545,17 +1569,17 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>1</v>
+      <c r="A51" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
       </c>
       <c r="C51" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D51" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E51" s="4">
         <f>B51*C51/D51</f>
@@ -1564,16 +1588,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
       </c>
       <c r="C52" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D52" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E52" s="4">
         <f>B52*C52/D52</f>
@@ -1582,13 +1606,13 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
       </c>
       <c r="C53" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D53" s="1">
         <v>3</v>
@@ -1600,13 +1624,13 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
       </c>
       <c r="C54" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D54" s="1">
         <v>3</v>
@@ -1617,8 +1641,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
-        <v>12</v>
+      <c r="A55" t="s">
+        <v>40</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -1627,7 +1651,7 @@
         <v>4</v>
       </c>
       <c r="D55" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E55" s="4">
         <f>B55*C55/D55</f>
@@ -1635,8 +1659,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>19</v>
+      <c r="A56" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -1645,7 +1669,7 @@
         <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E56" s="4">
         <f>B56*C56/D56</f>
@@ -1653,17 +1677,17 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
-        <v>18</v>
+      <c r="A57" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
       </c>
       <c r="C57" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D57" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E57" s="4">
         <f>B57*C57/D57</f>
@@ -1671,17 +1695,17 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="6" t="s">
-        <v>63</v>
+      <c r="A58" t="s">
+        <v>17</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D58" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E58" s="4">
         <f>B58*C58/D58</f>
@@ -1690,16 +1714,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>46</v>
+        <v>1</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D59" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E59" s="4">
         <f>B59*C59/D59</f>
@@ -1707,17 +1731,17 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="3" t="s">
-        <v>43</v>
+      <c r="A60" t="s">
+        <v>9</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="C60" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D60" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E60" s="4">
         <f>B60*C60/D60</f>
@@ -1726,7 +1750,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -1735,7 +1759,7 @@
         <v>3</v>
       </c>
       <c r="D61" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E61" s="4">
         <f>B61*C61/D61</f>
@@ -1744,7 +1768,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -1753,7 +1777,7 @@
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E62" s="4">
         <f>B62*C62/D62</f>
@@ -1761,14 +1785,14 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>62</v>
+      <c r="A63" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
       </c>
       <c r="C63" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D63" s="1">
         <v>4</v>
@@ -1780,16 +1804,16 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
       </c>
       <c r="C64" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D64" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E64" s="4">
         <f>B64*C64/D64</f>
@@ -1797,17 +1821,17 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>48</v>
+      <c r="A65" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
       </c>
       <c r="C65" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D65" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E65" s="4">
         <f>B65*C65/D65</f>
@@ -1815,26 +1839,170 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
-        <v>41</v>
+      <c r="A66" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B66" s="1">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C66" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D66" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E66" s="4">
         <f>B66*C66/D66</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>46</v>
+      </c>
+      <c r="B67" s="1">
+        <v>0</v>
+      </c>
+      <c r="C67" s="1">
+        <v>4</v>
+      </c>
+      <c r="D67" s="1">
+        <v>5</v>
+      </c>
+      <c r="E67" s="4">
+        <f>B67*C67/D67</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68" s="1">
+        <v>0</v>
+      </c>
+      <c r="C68" s="1">
+        <v>3</v>
+      </c>
+      <c r="D68" s="1">
+        <v>4</v>
+      </c>
+      <c r="E68" s="4">
+        <f>B68*C68/D68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" s="1">
+        <v>0</v>
+      </c>
+      <c r="C69" s="1">
+        <v>3</v>
+      </c>
+      <c r="D69" s="1">
+        <v>4</v>
+      </c>
+      <c r="E69" s="4">
+        <f>B69*C69/D69</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" s="1">
+        <v>0</v>
+      </c>
+      <c r="C70" s="1">
+        <v>3</v>
+      </c>
+      <c r="D70" s="1">
+        <v>4</v>
+      </c>
+      <c r="E70" s="4">
+        <f>B70*C70/D70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="1">
+        <v>0</v>
+      </c>
+      <c r="C71" s="1">
+        <v>3</v>
+      </c>
+      <c r="D71" s="1">
+        <v>4</v>
+      </c>
+      <c r="E71" s="4">
+        <f>B71*C71/D71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" s="1">
+        <v>0</v>
+      </c>
+      <c r="C72" s="1">
+        <v>2</v>
+      </c>
+      <c r="D72" s="1">
+        <v>3</v>
+      </c>
+      <c r="E72" s="4">
+        <f>B72*C72/D72</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" s="1">
+        <v>0</v>
+      </c>
+      <c r="C73" s="1">
+        <v>2</v>
+      </c>
+      <c r="D73" s="1">
+        <v>3</v>
+      </c>
+      <c r="E73" s="4">
+        <f>B73*C73/D73</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B74" s="1">
+        <v>-1</v>
+      </c>
+      <c r="C74" s="1">
+        <v>4</v>
+      </c>
+      <c r="D74" s="1">
+        <v>2</v>
+      </c>
+      <c r="E74" s="4">
+        <f>B74*C74/D74</f>
         <v>-2</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E66">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E74">
       <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
473 Additional commands added.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD30F0E-457B-4D8F-A3C6-397626608DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A0451D-1CF4-4C42-927B-4913F2AB6628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2640" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B76"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <f>B2*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">B2*C2/D2</f>
         <v>5</v>
       </c>
     </row>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <f>B3*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <f>B4*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4">
-        <f>B5*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="4">
-        <f>B6*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -796,7 +796,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="4">
-        <f>B7*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="4">
-        <f>B8*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -832,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="4">
-        <f>B9*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4">
-        <f>B10*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -868,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="4">
-        <f>B11*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -886,7 +886,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="4">
-        <f>B12*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -904,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="4">
-        <f>B13*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -922,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="4">
-        <f>B14*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -940,7 +940,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="4">
-        <f>B15*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -958,7 +958,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="4">
-        <f>B16*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="4">
-        <f>B17*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -994,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="4">
-        <f>B18*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="4">
-        <f>B19*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="4">
-        <f>B20*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="4">
-        <f>B21*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="4">
-        <f>B22*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="4">
-        <f>B23*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="4">
-        <f>B24*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <f>B25*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f>B26*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f>B27*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="4">
-        <f>B28*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="4">
-        <f>B29*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="4">
-        <f>B30*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="4">
-        <f>B31*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="4">
-        <f>B32*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="4">
-        <f>B33*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="4">
-        <f>B34*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="1">B34*C34/D34</f>
         <v>0</v>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="4">
-        <f>B35*C35/D35</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="4">
-        <f>B36*C36/D36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1327,17 +1327,17 @@
         <v>10</v>
       </c>
       <c r="B37" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C37" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E37" s="4">
-        <f>B37*C37/D37</f>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>2.5</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1354,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="4">
-        <f>B38*C38/D38</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="4">
-        <f>B39*C39/D39</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1390,7 +1390,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="4">
-        <f>B40*C40/D40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1408,7 +1408,7 @@
         <v>3</v>
       </c>
       <c r="E41" s="4">
-        <f>B41*C41/D41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="4">
-        <f>B42*C42/D42</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1444,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="4">
-        <f>B43*C43/D43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="4">
-        <f>B44*C44/D44</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="4">
-        <f>B45*C45/D45</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1498,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="4">
-        <f>B46*C46/D46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="4">
-        <f>B47*C47/D47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1534,7 +1534,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="4">
-        <f>B48*C48/D48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="E49" s="4">
-        <f>B49*C49/D49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="4">
-        <f>B50*C50/D50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="4">
-        <f>B51*C51/D51</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="4">
-        <f>B52*C52/D52</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="4">
-        <f>B53*C53/D53</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="4">
-        <f>B54*C54/D54</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="4">
-        <f>B55*C55/D55</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="4">
-        <f>B56*C56/D56</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="E57" s="4">
-        <f>B57*C57/D57</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1714,7 +1714,7 @@
         <v>3</v>
       </c>
       <c r="E58" s="4">
-        <f>B58*C58/D58</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1732,7 +1732,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="4">
-        <f>B59*C59/D59</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
         <v>4</v>
       </c>
       <c r="E60" s="4">
-        <f>B60*C60/D60</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="E61" s="4">
-        <f>B61*C61/D61</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="4">
-        <f>B62*C62/D62</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="4">
-        <f>B63*C63/D63</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="E64" s="4">
-        <f>B64*C64/D64</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="E65" s="4">
-        <f>B65*C65/D65</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1858,7 +1858,7 @@
         <v>4</v>
       </c>
       <c r="E66" s="4">
-        <f>B66*C66/D66</f>
+        <f t="shared" ref="E66:E97" si="2">B66*C66/D66</f>
         <v>0</v>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
         <v>5</v>
       </c>
       <c r="E67" s="4">
-        <f>B67*C67/D67</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1894,7 +1894,7 @@
         <v>3</v>
       </c>
       <c r="E68" s="4">
-        <f>B68*C68/D68</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
         <v>5</v>
       </c>
       <c r="E69" s="4">
-        <f>B69*C69/D69</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1930,7 +1930,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="4">
-        <f>B70*C70/D70</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
         <v>4</v>
       </c>
       <c r="E71" s="4">
-        <f>B71*C71/D71</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
         <v>4</v>
       </c>
       <c r="E72" s="4">
-        <f>B72*C72/D72</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="E73" s="4">
-        <f>B73*C73/D73</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2002,7 +2002,7 @@
         <v>4</v>
       </c>
       <c r="E74" s="4">
-        <f>B74*C74/D74</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2020,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="4">
-        <f>B75*C75/D75</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="E76" s="4">
-        <f>B76*C76/D76</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Time-fix implemented: time is now in minutes.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A0451D-1CF4-4C42-927B-4913F2AB6628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D683FA49-1E2C-4122-9033-7AE673FDEEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2640" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -662,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,7 +706,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <f t="shared" ref="E2:E33" si="0">B2*C2/D2</f>
+        <f>B2*C2/D2</f>
         <v>5</v>
       </c>
     </row>
@@ -724,7 +724,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" si="0"/>
+        <f>B3*C3/D3</f>
         <v>4</v>
       </c>
     </row>
@@ -742,7 +742,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" si="0"/>
+        <f>B4*C4/D4</f>
         <v>3</v>
       </c>
     </row>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="0"/>
+        <f>B5*C5/D5</f>
         <v>3</v>
       </c>
     </row>
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" si="0"/>
+        <f>B6*C6/D6</f>
         <v>2</v>
       </c>
     </row>
@@ -796,7 +796,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="4">
-        <f t="shared" si="0"/>
+        <f>B7*C7/D7</f>
         <v>2</v>
       </c>
     </row>
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="4">
-        <f t="shared" si="0"/>
+        <f>B8*C8/D8</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -832,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="4">
-        <f t="shared" si="0"/>
+        <f>B9*C9/D9</f>
         <v>1.5</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4">
-        <f t="shared" si="0"/>
+        <f>B10*C10/D10</f>
         <v>1.5</v>
       </c>
     </row>
@@ -868,7 +868,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="4">
-        <f t="shared" si="0"/>
+        <f>B11*C11/D11</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
@@ -886,7 +886,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" si="0"/>
+        <f>B12*C12/D12</f>
         <v>1</v>
       </c>
     </row>
@@ -904,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="0"/>
+        <f>B13*C13/D13</f>
         <v>1</v>
       </c>
     </row>
@@ -922,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="0"/>
+        <f>B14*C14/D14</f>
         <v>1</v>
       </c>
     </row>
@@ -940,7 +940,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="0"/>
+        <f>B15*C15/D15</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -958,7 +958,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="4">
-        <f t="shared" si="0"/>
+        <f>B16*C16/D16</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -976,7 +976,7 @@
         <v>3</v>
       </c>
       <c r="E17" s="4">
-        <f t="shared" si="0"/>
+        <f>B17*C17/D17</f>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -994,13 +994,13 @@
         <v>4</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="0"/>
+        <f>B18*C18/D18</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -1009,29 +1009,29 @@
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="0"/>
-        <v>0.33333333333333331</v>
+        <f>B19*C19/D19</f>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="B20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
+        <f>B20*C20/D20</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1048,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="0"/>
+        <f>B21*C21/D21</f>
         <v>0</v>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="0"/>
+        <f>B22*C22/D22</f>
         <v>0</v>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="0"/>
+        <f>B23*C23/D23</f>
         <v>0</v>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="4">
-        <f t="shared" si="0"/>
+        <f>B24*C24/D24</f>
         <v>0</v>
       </c>
     </row>
@@ -1120,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" si="0"/>
+        <f>B25*C25/D25</f>
         <v>0</v>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" si="0"/>
+        <f>B26*C26/D26</f>
         <v>0</v>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" si="0"/>
+        <f>B27*C27/D27</f>
         <v>0</v>
       </c>
     </row>
@@ -1174,7 +1174,7 @@
         <v>1</v>
       </c>
       <c r="E28" s="4">
-        <f t="shared" si="0"/>
+        <f>B28*C28/D28</f>
         <v>0</v>
       </c>
     </row>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" si="0"/>
+        <f>B29*C29/D29</f>
         <v>0</v>
       </c>
     </row>
@@ -1210,7 +1210,7 @@
         <v>1</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" si="0"/>
+        <f>B30*C30/D30</f>
         <v>0</v>
       </c>
     </row>
@@ -1228,7 +1228,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" si="0"/>
+        <f>B31*C31/D31</f>
         <v>0</v>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="4">
-        <f t="shared" si="0"/>
+        <f>B32*C32/D32</f>
         <v>0</v>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="E33" s="4">
-        <f t="shared" si="0"/>
+        <f>B33*C33/D33</f>
         <v>0</v>
       </c>
     </row>
@@ -1282,7 +1282,7 @@
         <v>1</v>
       </c>
       <c r="E34" s="4">
-        <f t="shared" ref="E34:E65" si="1">B34*C34/D34</f>
+        <f>B34*C34/D34</f>
         <v>0</v>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="4">
-        <f t="shared" si="1"/>
+        <f>B35*C35/D35</f>
         <v>0</v>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="4">
-        <f t="shared" si="1"/>
+        <f>B36*C36/D36</f>
         <v>0</v>
       </c>
     </row>
@@ -1327,7 +1327,7 @@
         <v>10</v>
       </c>
       <c r="B37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37" s="1">
         <v>5</v>
@@ -1336,8 +1336,8 @@
         <v>2</v>
       </c>
       <c r="E37" s="4">
-        <f t="shared" si="1"/>
-        <v>2.5</v>
+        <f>B37*C37/D37</f>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1354,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="4">
-        <f t="shared" si="1"/>
+        <f>B38*C38/D38</f>
         <v>0</v>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="4">
-        <f t="shared" si="1"/>
+        <f>B39*C39/D39</f>
         <v>0</v>
       </c>
     </row>
@@ -1390,7 +1390,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" si="1"/>
+        <f>B40*C40/D40</f>
         <v>0</v>
       </c>
     </row>
@@ -1408,7 +1408,7 @@
         <v>3</v>
       </c>
       <c r="E41" s="4">
-        <f t="shared" si="1"/>
+        <f>B41*C41/D41</f>
         <v>0</v>
       </c>
     </row>
@@ -1426,7 +1426,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="4">
-        <f t="shared" si="1"/>
+        <f>B42*C42/D42</f>
         <v>0</v>
       </c>
     </row>
@@ -1444,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="4">
-        <f t="shared" si="1"/>
+        <f>B43*C43/D43</f>
         <v>0</v>
       </c>
     </row>
@@ -1462,7 +1462,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="4">
-        <f t="shared" si="1"/>
+        <f>B44*C44/D44</f>
         <v>0</v>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="4">
-        <f t="shared" si="1"/>
+        <f>B45*C45/D45</f>
         <v>0</v>
       </c>
     </row>
@@ -1498,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="4">
-        <f t="shared" si="1"/>
+        <f>B46*C46/D46</f>
         <v>0</v>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="4">
-        <f t="shared" si="1"/>
+        <f>B47*C47/D47</f>
         <v>0</v>
       </c>
     </row>
@@ -1534,7 +1534,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="4">
-        <f t="shared" si="1"/>
+        <f>B48*C48/D48</f>
         <v>0</v>
       </c>
     </row>
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="E49" s="4">
-        <f t="shared" si="1"/>
+        <f>B49*C49/D49</f>
         <v>0</v>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="4">
-        <f t="shared" si="1"/>
+        <f>B50*C50/D50</f>
         <v>0</v>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="4">
-        <f t="shared" si="1"/>
+        <f>B51*C51/D51</f>
         <v>0</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="4">
-        <f t="shared" si="1"/>
+        <f>B52*C52/D52</f>
         <v>0</v>
       </c>
     </row>
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="4">
-        <f t="shared" si="1"/>
+        <f>B53*C53/D53</f>
         <v>0</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="4">
-        <f t="shared" si="1"/>
+        <f>B54*C54/D54</f>
         <v>0</v>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="4">
-        <f t="shared" si="1"/>
+        <f>B55*C55/D55</f>
         <v>0</v>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="4">
-        <f t="shared" si="1"/>
+        <f>B56*C56/D56</f>
         <v>0</v>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="E57" s="4">
-        <f t="shared" si="1"/>
+        <f>B57*C57/D57</f>
         <v>0</v>
       </c>
     </row>
@@ -1714,7 +1714,7 @@
         <v>3</v>
       </c>
       <c r="E58" s="4">
-        <f t="shared" si="1"/>
+        <f>B58*C58/D58</f>
         <v>0</v>
       </c>
     </row>
@@ -1732,7 +1732,7 @@
         <v>4</v>
       </c>
       <c r="E59" s="4">
-        <f t="shared" si="1"/>
+        <f>B59*C59/D59</f>
         <v>0</v>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
         <v>4</v>
       </c>
       <c r="E60" s="4">
-        <f t="shared" si="1"/>
+        <f>B60*C60/D60</f>
         <v>0</v>
       </c>
     </row>
@@ -1768,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="E61" s="4">
-        <f t="shared" si="1"/>
+        <f>B61*C61/D61</f>
         <v>0</v>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
         <v>1</v>
       </c>
       <c r="E62" s="4">
-        <f t="shared" si="1"/>
+        <f>B62*C62/D62</f>
         <v>0</v>
       </c>
     </row>
@@ -1804,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="4">
-        <f t="shared" si="1"/>
+        <f>B63*C63/D63</f>
         <v>0</v>
       </c>
     </row>
@@ -1822,7 +1822,7 @@
         <v>3</v>
       </c>
       <c r="E64" s="4">
-        <f t="shared" si="1"/>
+        <f>B64*C64/D64</f>
         <v>0</v>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
         <v>4</v>
       </c>
       <c r="E65" s="4">
-        <f t="shared" si="1"/>
+        <f>B65*C65/D65</f>
         <v>0</v>
       </c>
     </row>
@@ -1858,7 +1858,7 @@
         <v>4</v>
       </c>
       <c r="E66" s="4">
-        <f t="shared" ref="E66:E97" si="2">B66*C66/D66</f>
+        <f>B66*C66/D66</f>
         <v>0</v>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
         <v>5</v>
       </c>
       <c r="E67" s="4">
-        <f t="shared" si="2"/>
+        <f>B67*C67/D67</f>
         <v>0</v>
       </c>
     </row>
@@ -1894,7 +1894,7 @@
         <v>3</v>
       </c>
       <c r="E68" s="4">
-        <f t="shared" si="2"/>
+        <f>B68*C68/D68</f>
         <v>0</v>
       </c>
     </row>
@@ -1912,7 +1912,7 @@
         <v>5</v>
       </c>
       <c r="E69" s="4">
-        <f t="shared" si="2"/>
+        <f>B69*C69/D69</f>
         <v>0</v>
       </c>
     </row>
@@ -1930,7 +1930,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="4">
-        <f t="shared" si="2"/>
+        <f>B70*C70/D70</f>
         <v>0</v>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
         <v>4</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="2"/>
+        <f>B71*C71/D71</f>
         <v>0</v>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
         <v>4</v>
       </c>
       <c r="E72" s="4">
-        <f t="shared" si="2"/>
+        <f>B72*C72/D72</f>
         <v>0</v>
       </c>
     </row>
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="E73" s="4">
-        <f t="shared" si="2"/>
+        <f>B73*C73/D73</f>
         <v>0</v>
       </c>
     </row>
@@ -2002,7 +2002,7 @@
         <v>4</v>
       </c>
       <c r="E74" s="4">
-        <f t="shared" si="2"/>
+        <f>B74*C74/D74</f>
         <v>0</v>
       </c>
     </row>
@@ -2020,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="E75" s="4">
-        <f t="shared" si="2"/>
+        <f>B75*C75/D75</f>
         <v>0</v>
       </c>
     </row>
@@ -2038,7 +2038,7 @@
         <v>3</v>
       </c>
       <c r="E76" s="4">
-        <f t="shared" si="2"/>
+        <f>B76*C76/D76</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
3900 Additional functions and FPH calibration
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D683FA49-1E2C-4122-9033-7AE673FDEEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCBAF22-0737-4B5D-BED6-FE2FF6E4F826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2640" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,9 +246,6 @@
     <t>Move autoprofile checks to insturment files</t>
   </si>
   <si>
-    <t>Rotation stage</t>
-  </si>
-  <si>
     <t>mK and uK self-heating checks</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>Instument files refer to external cal source</t>
+  </si>
+  <si>
+    <t>Rotation and translation stages</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
   <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,7 +694,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -706,13 +706,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="4">
-        <f>B2*C2/D2</f>
+        <f t="shared" ref="E2:E33" si="0">B2*C2/D2</f>
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -724,13 +724,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="4">
-        <f>B3*C3/D3</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -742,13 +742,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="4">
-        <f>B4*C4/D4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -760,7 +760,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="4">
-        <f>B5*C5/D5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -772,31 +772,31 @@
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4">
-        <f>B6*C6/D6</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" s="4">
-        <f>B7*C7/D7</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
@@ -814,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="4">
-        <f>B8*C8/D8</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666667</v>
       </c>
     </row>
@@ -832,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="4">
-        <f>B9*C9/D9</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4">
-        <f>B10*C10/D10</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
@@ -868,31 +868,31 @@
         <v>3</v>
       </c>
       <c r="E11" s="4">
-        <f>B11*C11/D11</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E12" s="4">
-        <f>B12*C12/D12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -904,25 +904,25 @@
         <v>3</v>
       </c>
       <c r="E13" s="4">
-        <f>B13*C13/D13</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4">
-        <f>B14*C14/D14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -940,7 +940,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="4">
-        <f>B15*C15/D15</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -958,7 +958,7 @@
         <v>3</v>
       </c>
       <c r="E16" s="4">
-        <f>B16*C16/D16</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
@@ -976,13 +976,13 @@
         <v>3</v>
       </c>
       <c r="E17" s="4">
-        <f>B17*C17/D17</f>
+        <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1">
         <v>1</v>
@@ -994,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="E18" s="4">
-        <f>B18*C18/D18</f>
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
@@ -1012,31 +1012,31 @@
         <v>5</v>
       </c>
       <c r="E19" s="4">
-        <f>B19*C19/D19</f>
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="4">
-        <f>B20*C20/D20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1048,13 +1048,13 @@
         <v>1</v>
       </c>
       <c r="E21" s="4">
-        <f>B21*C21/D21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1066,13 +1066,13 @@
         <v>1</v>
       </c>
       <c r="E22" s="4">
-        <f>B22*C22/D22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -1084,13 +1084,13 @@
         <v>1</v>
       </c>
       <c r="E23" s="4">
-        <f>B23*C23/D23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1102,31 +1102,31 @@
         <v>1</v>
       </c>
       <c r="E24" s="4">
-        <f>B24*C24/D24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <f>B25*C25/D25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -1138,13 +1138,13 @@
         <v>1</v>
       </c>
       <c r="E26" s="4">
-        <f>B26*C26/D26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1156,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="4">
-        <f>B27*C27/D27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1174,13 +1174,13 @@
         <v>1</v>
       </c>
       <c r="E28" s="4">
-        <f>B28*C28/D28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>54</v>
+      <c r="A29" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1192,31 +1192,31 @@
         <v>1</v>
       </c>
       <c r="E29" s="4">
-        <f>B29*C29/D29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
+      <c r="A30" t="s">
+        <v>53</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
       <c r="C30" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
       </c>
       <c r="E30" s="4">
-        <f>B30*C30/D30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -1228,13 +1228,13 @@
         <v>1</v>
       </c>
       <c r="E31" s="4">
-        <f>B31*C31/D31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1246,13 +1246,13 @@
         <v>1</v>
       </c>
       <c r="E32" s="4">
-        <f>B32*C32/D32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -1264,25 +1264,25 @@
         <v>1</v>
       </c>
       <c r="E33" s="4">
-        <f>B33*C33/D33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
       </c>
       <c r="E34" s="4">
-        <f>B34*C34/D34</f>
+        <f t="shared" ref="E34:E65" si="1">B34*C34/D34</f>
         <v>0</v>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="4">
-        <f>B35*C35/D35</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1318,7 +1318,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="4">
-        <f>B36*C36/D36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="4">
-        <f>B37*C37/D37</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1354,7 +1354,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="4">
-        <f>B38*C38/D38</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1372,7 +1372,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="4">
-        <f>B39*C39/D39</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1390,31 +1390,31 @@
         <v>2</v>
       </c>
       <c r="E40" s="4">
-        <f>B40*C40/D40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
-        <v>44</v>
+      <c r="A41" t="s">
+        <v>58</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
       </c>
       <c r="C41" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D41" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="4">
-        <f>B41*C41/D41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>58</v>
+      <c r="A42" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -1426,13 +1426,13 @@
         <v>2</v>
       </c>
       <c r="E42" s="4">
-        <f>B42*C42/D42</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -1444,13 +1444,13 @@
         <v>2</v>
       </c>
       <c r="E43" s="4">
-        <f>B43*C43/D43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
-        <v>33</v>
+      <c r="A44" t="s">
+        <v>16</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -1462,13 +1462,13 @@
         <v>2</v>
       </c>
       <c r="E44" s="4">
-        <f>B44*C44/D44</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>16</v>
+      <c r="A45" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -1480,25 +1480,25 @@
         <v>2</v>
       </c>
       <c r="E45" s="4">
-        <f>B45*C45/D45</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D46" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E46" s="4">
-        <f>B46*C46/D46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
         <v>3</v>
       </c>
       <c r="E47" s="4">
-        <f>B47*C47/D47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1534,7 +1534,7 @@
         <v>3</v>
       </c>
       <c r="E48" s="4">
-        <f>B48*C48/D48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="E49" s="4">
-        <f>B49*C49/D49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
         <v>3</v>
       </c>
       <c r="E50" s="4">
-        <f>B50*C50/D50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1588,7 +1588,7 @@
         <v>3</v>
       </c>
       <c r="E51" s="4">
-        <f>B51*C51/D51</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="4">
-        <f>B52*C52/D52</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1624,7 +1624,7 @@
         <v>3</v>
       </c>
       <c r="E53" s="4">
-        <f>B53*C53/D53</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
         <v>3</v>
       </c>
       <c r="E54" s="4">
-        <f>B54*C54/D54</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="E55" s="4">
-        <f>B55*C55/D55</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1678,7 +1678,7 @@
         <v>3</v>
       </c>
       <c r="E56" s="4">
-        <f>B56*C56/D56</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="E57" s="4">
-        <f>B57*C57/D57</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1714,49 +1714,49 @@
         <v>3</v>
       </c>
       <c r="E58" s="4">
-        <f>B58*C58/D58</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D59" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E59" s="4">
-        <f>B59*C59/D59</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="C60" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D60" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E60" s="4">
-        <f>B60*C60/D60</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -1768,103 +1768,103 @@
         <v>3</v>
       </c>
       <c r="E61" s="4">
-        <f>B61*C61/D61</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>9</v>
+      <c r="A62" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
       </c>
       <c r="C62" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E62" s="4">
-        <f>B62*C62/D62</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
       </c>
       <c r="C63" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63" s="1">
         <v>3</v>
       </c>
       <c r="E63" s="4">
-        <f>B63*C63/D63</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
       </c>
       <c r="C64" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D64" s="1">
         <v>3</v>
       </c>
       <c r="E64" s="4">
-        <f>B64*C64/D64</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="2" t="s">
-        <v>12</v>
+      <c r="A65" t="s">
+        <v>72</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
       </c>
       <c r="C65" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D65" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E65" s="4">
-        <f>B65*C65/D65</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
       </c>
       <c r="C66" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D66" s="1">
         <v>4</v>
       </c>
       <c r="E66" s="4">
-        <f>B66*C66/D66</f>
+        <f t="shared" ref="E66:E97" si="2">B66*C66/D66</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="3" t="s">
-        <v>18</v>
+      <c r="A67" t="s">
+        <v>1</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
@@ -1873,34 +1873,34 @@
         <v>5</v>
       </c>
       <c r="D67" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E67" s="4">
-        <f>B67*C67/D67</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="6" t="s">
-        <v>63</v>
+      <c r="A68" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
       </c>
       <c r="C68" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D68" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E68" s="4">
-        <f>B68*C68/D68</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
@@ -1909,10 +1909,10 @@
         <v>4</v>
       </c>
       <c r="D69" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E69" s="4">
-        <f>B69*C69/D69</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1930,7 +1930,7 @@
         <v>4</v>
       </c>
       <c r="E70" s="4">
-        <f>B70*C70/D70</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1948,7 +1948,7 @@
         <v>4</v>
       </c>
       <c r="E71" s="4">
-        <f>B71*C71/D71</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
         <v>4</v>
       </c>
       <c r="E72" s="4">
-        <f>B72*C72/D72</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="E73" s="4">
-        <f>B73*C73/D73</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2002,43 +2002,43 @@
         <v>4</v>
       </c>
       <c r="E74" s="4">
-        <f>B74*C74/D74</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>61</v>
+      <c r="A75" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
       </c>
       <c r="C75" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D75" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E75" s="4">
-        <f>B75*C75/D75</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
       </c>
       <c r="C76" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D76" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E76" s="4">
-        <f>B76*C76/D76</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Hash listing and cal checking (requires bypass)
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05BD8EEE-24B6-4B9C-9AB8-D2D6C6080A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80749EB5-654C-493E-A717-B1290E795653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2640" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Name</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Rotation and translation stages</t>
+  </si>
+  <si>
+    <t>Open files from specific folders</t>
   </si>
 </sst>
 </file>
@@ -657,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,7 +766,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -781,7 +784,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -798,44 +801,44 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>49</v>
+      <c r="A8" t="s">
+        <v>45</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="4">
         <f>B8*C8/D8</f>
-        <v>1.3333333333333333</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>68</v>
+      <c r="A9" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="4">
         <f>B9*C9/D9</f>
-        <v>1</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -853,7 +856,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -871,16 +874,16 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" s="4">
         <f>B12*C12/D12</f>
@@ -889,7 +892,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
@@ -898,34 +901,34 @@
         <v>3</v>
       </c>
       <c r="D13" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E13" s="4">
         <f>B13*C13/D13</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
-        <v>28</v>
+      <c r="A14" t="s">
+        <v>66</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4">
         <f>B14*C14/D14</f>
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -942,8 +945,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>65</v>
+      <c r="A16" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -961,52 +964,52 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="4">
         <f>B17*C17/D17</f>
-        <v>0.2</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>78</v>
+      <c r="A18" t="s">
+        <v>51</v>
       </c>
       <c r="B18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E18" s="4">
         <f>B18*C18/D18</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>59</v>
+      <c r="A19" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E19" s="4">
         <f>B19*C19/D19</f>
@@ -1015,7 +1018,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1033,7 +1036,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1051,7 +1054,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1069,7 +1072,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -1087,13 +1090,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -1105,7 +1108,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1123,7 +1126,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -1141,7 +1144,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>54</v>
+        <v>4</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1158,8 +1161,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>30</v>
+      <c r="A28" t="s">
+        <v>54</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1176,14 +1179,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>53</v>
+      <c r="A29" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1195,7 +1198,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1213,7 +1216,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -1231,7 +1234,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1249,13 +1252,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D33" s="1">
         <v>1</v>
@@ -1267,16 +1270,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="4">
         <f>B34*C34/D34</f>
@@ -1285,7 +1288,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -1303,7 +1306,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -1320,14 +1323,14 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
-        <v>23</v>
+      <c r="A37" t="s">
+        <v>10</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
       </c>
       <c r="C37" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D37" s="1">
         <v>2</v>
@@ -1338,8 +1341,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>56</v>
+      <c r="A38" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -1356,8 +1359,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
-        <v>41</v>
+      <c r="A39" t="s">
+        <v>56</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -1374,14 +1377,14 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>58</v>
+      <c r="A40" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
       </c>
       <c r="C40" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1">
         <v>2</v>
@@ -1392,8 +1395,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
-        <v>39</v>
+      <c r="A41" t="s">
+        <v>58</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -1411,7 +1414,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -1428,8 +1431,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>16</v>
+      <c r="A43" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -1446,8 +1449,8 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="3" t="s">
-        <v>34</v>
+      <c r="A44" t="s">
+        <v>16</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -1465,16 +1468,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
       </c>
       <c r="C45" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E45" s="4">
         <f>B45*C45/D45</f>
@@ -1482,14 +1485,14 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>31</v>
+      <c r="A46" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D46" s="1">
         <v>3</v>
@@ -1501,7 +1504,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -1519,7 +1522,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1555,7 +1558,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -1573,7 +1576,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -1590,8 +1593,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>21</v>
+      <c r="A52" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -1609,7 +1612,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1627,7 +1630,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -1645,7 +1648,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -1662,8 +1665,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
-        <v>47</v>
+      <c r="A56" t="s">
+        <v>40</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -1680,8 +1683,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
-        <v>13</v>
+      <c r="A57" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
@@ -1698,14 +1701,14 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>75</v>
+      <c r="A58" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D58" s="1">
         <v>3</v>
@@ -1717,7 +1720,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
@@ -1735,7 +1738,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
@@ -1752,8 +1755,8 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="6" t="s">
-        <v>62</v>
+      <c r="A61" t="s">
+        <v>35</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -1770,14 +1773,14 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>60</v>
+      <c r="A62" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
       </c>
       <c r="C62" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
         <v>3</v>
@@ -1789,7 +1792,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
@@ -1807,13 +1810,13 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
       </c>
       <c r="C64" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D64" s="1">
         <v>3</v>
@@ -1825,16 +1828,16 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
       </c>
       <c r="C65" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D65" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E65" s="4">
         <f>B65*C65/D65</f>
@@ -1843,7 +1846,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
@@ -1860,14 +1863,14 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" s="2" t="s">
-        <v>12</v>
+      <c r="A67" t="s">
+        <v>1</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
       </c>
       <c r="C67" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D67" s="1">
         <v>4</v>
@@ -1878,8 +1881,8 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>19</v>
+      <c r="A68" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
@@ -1897,13 +1900,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
       </c>
       <c r="C69" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D69" s="1">
         <v>4</v>
@@ -1914,8 +1917,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" s="3" t="s">
-        <v>43</v>
+      <c r="A70" t="s">
+        <v>67</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -1932,8 +1935,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>32</v>
+      <c r="A71" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
@@ -1951,7 +1954,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -1969,7 +1972,7 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>20</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
@@ -1986,17 +1989,17 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" s="3" t="s">
-        <v>18</v>
+      <c r="A74" t="s">
+        <v>61</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
       </c>
       <c r="C74" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D74" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E74" s="4">
         <f>B74*C74/D74</f>
@@ -2004,14 +2007,14 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>46</v>
+      <c r="A75" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
       </c>
       <c r="C75" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D75" s="1">
         <v>5</v>
@@ -2021,14 +2024,32 @@
         <v>0</v>
       </c>
     </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>46</v>
+      </c>
+      <c r="B76" s="1">
+        <v>0</v>
+      </c>
+      <c r="C76" s="1">
+        <v>4</v>
+      </c>
+      <c r="D76" s="1">
+        <v>5</v>
+      </c>
+      <c r="E76" s="4">
+        <f>B76*C76/D76</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E75">
-      <sortCondition descending="1" ref="E1:E11"/>
+  <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E76">
+      <sortCondition descending="1" ref="E1:E12"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E10">
-    <sortCondition descending="1" ref="E2:E10"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E11">
+    <sortCondition descending="1" ref="E3:E11"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="colorScale" priority="3">
@@ -2042,7 +2063,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:D46">
+  <conditionalFormatting sqref="D35:D47">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -2052,28 +2073,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31:C46">
+  <conditionalFormatting sqref="C32:C47">
     <cfRule type="colorScale" priority="55">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2083,7 +2084,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2093,7 +2094,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2103,7 +2104,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2113,7 +2114,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2123,7 +2124,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2133,7 +2134,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2143,7 +2144,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2153,7 +2154,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2163,7 +2164,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2173,7 +2174,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2183,7 +2184,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2193,7 +2194,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2203,7 +2204,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2213,7 +2214,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2223,6 +2224,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2274,7 +2295,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D35">
+  <conditionalFormatting sqref="D3:D36">
     <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
@@ -2284,7 +2305,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C30">
+  <conditionalFormatting sqref="C3:C31">
     <cfRule type="colorScale" priority="89">
       <colorScale>
         <cfvo type="min"/>
@@ -2294,7 +2315,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B75">
+  <conditionalFormatting sqref="B3:B76">
     <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
@@ -2314,7 +2335,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E46">
+  <conditionalFormatting sqref="E2:E47">
     <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
@@ -2326,7 +2347,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C46">
+  <conditionalFormatting sqref="C3:C47">
     <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min"/>
@@ -2336,7 +2357,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D46">
+  <conditionalFormatting sqref="D3:D47">
     <cfRule type="colorScale" priority="99">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Added Met-Service devices to HP instrument file
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80749EB5-654C-493E-A717-B1290E795653}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47F4584-9AE9-4E46-B4C0-C3BDB56A5633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="79">
   <si>
     <t>Name</t>
   </si>
@@ -231,15 +231,9 @@
     <t>"Writing" on screen</t>
   </si>
   <si>
-    <t>Save profile?</t>
-  </si>
-  <si>
     <t>Setup.py?</t>
   </si>
   <si>
-    <t>Fix graph saving</t>
-  </si>
-  <si>
     <t>Move autoprofile checks to insturment files</t>
   </si>
   <si>
@@ -277,6 +271,9 @@
   </si>
   <si>
     <t>Open files from specific folders</t>
+  </si>
+  <si>
+    <t>Fix save interruption</t>
   </si>
 </sst>
 </file>
@@ -660,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -694,7 +691,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -712,7 +709,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -730,7 +727,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -748,25 +745,25 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="4">
         <f>B5*C5/D5</f>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -784,7 +781,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
@@ -801,44 +798,44 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>45</v>
+      <c r="A8" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
       </c>
       <c r="E8" s="4">
         <f>B8*C8/D8</f>
-        <v>1.6666666666666667</v>
+        <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>49</v>
+      <c r="A9" t="s">
+        <v>68</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="4">
         <f>B9*C9/D9</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -856,7 +853,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -874,61 +871,61 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E12" s="4">
         <f>B12*C12/D12</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>70</v>
+      <c r="A13" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="4">
         <f>B13*C13/D13</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>66</v>
+      <c r="A14" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14" s="4">
         <f>B14*C14/D14</f>
-        <v>0.75</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
-        <v>28</v>
+      <c r="A15" t="s">
+        <v>64</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
@@ -945,71 +942,71 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
-        <v>29</v>
+      <c r="A16" t="s">
+        <v>51</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E16" s="4">
         <f>B16*C16/D16</f>
-        <v>0.66666666666666663</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D17" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" s="4">
         <f>B17*C17/D17</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D18" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E18" s="4">
         <f>B18*C18/D18</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
-        <v>78</v>
+      <c r="A19" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E19" s="4">
         <f>B19*C19/D19</f>
@@ -1018,7 +1015,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
@@ -1036,7 +1033,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1054,13 +1051,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
       </c>
       <c r="C22" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1072,13 +1069,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
       </c>
       <c r="C23" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
@@ -1090,13 +1087,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>4</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
       </c>
       <c r="C24" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
@@ -1108,7 +1105,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1125,8 +1122,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>38</v>
+      <c r="A26" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -1144,13 +1141,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>4</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
       </c>
       <c r="C27" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
@@ -1162,13 +1159,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
       </c>
       <c r="C28" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1179,14 +1176,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
-        <v>30</v>
+      <c r="A29" t="s">
+        <v>3</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1198,7 +1195,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1216,16 +1213,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="4">
         <f>B31*C31/D31</f>
@@ -1234,16 +1231,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
       </c>
       <c r="C32" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" s="4">
         <f>B32*C32/D32</f>
@@ -1252,16 +1249,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="4">
         <f>B33*C33/D33</f>
@@ -1270,16 +1267,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" s="4">
         <f>B34*C34/D34</f>
@@ -1287,14 +1284,14 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>15</v>
+      <c r="A35" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D35" s="1">
         <v>2</v>
@@ -1306,13 +1303,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
       </c>
       <c r="C36" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1">
         <v>2</v>
@@ -1323,14 +1320,14 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>10</v>
+      <c r="A37" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
       </c>
       <c r="C37" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1">
         <v>2</v>
@@ -1341,17 +1338,17 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>23</v>
+      <c r="A38" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
       </c>
       <c r="C38" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D38" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="4">
         <f>B38*C38/D38</f>
@@ -1360,13 +1357,13 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
       </c>
       <c r="C39" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1">
         <v>2</v>
@@ -1378,13 +1375,13 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
       </c>
       <c r="C40" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1">
         <v>2</v>
@@ -1395,8 +1392,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>58</v>
+      <c r="A41" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -1413,8 +1410,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="3" t="s">
-        <v>39</v>
+      <c r="A42" t="s">
+        <v>16</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -1432,7 +1429,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -1449,17 +1446,17 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>16</v>
+      <c r="A44" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
       </c>
       <c r="C44" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D44" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E44" s="4">
         <f>B44*C44/D44</f>
@@ -1467,17 +1464,17 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="3" t="s">
-        <v>34</v>
+      <c r="A45" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
       </c>
       <c r="C45" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D45" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E45" s="4">
         <f>B45*C45/D45</f>
@@ -1485,14 +1482,14 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="3" t="s">
-        <v>44</v>
+      <c r="A46" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D46" s="1">
         <v>3</v>
@@ -1504,7 +1501,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -1522,7 +1519,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -1540,7 +1537,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1557,8 +1554,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>27</v>
+      <c r="A50" t="s">
+        <v>21</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -1575,8 +1572,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
-        <v>22</v>
+      <c r="A51" t="s">
+        <v>8</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -1593,8 +1590,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
-        <v>24</v>
+      <c r="A52" t="s">
+        <v>11</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -1612,7 +1609,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1629,8 +1626,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>8</v>
+      <c r="A54" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -1647,8 +1644,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>11</v>
+      <c r="A55" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -1666,16 +1663,16 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>17</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D56" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E56" s="4">
         <f>B56*C56/D56</f>
@@ -1683,17 +1680,17 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="3" t="s">
-        <v>47</v>
+      <c r="A57" t="s">
+        <v>1</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
       </c>
       <c r="C57" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D57" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E57" s="4">
         <f>B57*C57/D57</f>
@@ -1701,17 +1698,17 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
-        <v>13</v>
+      <c r="A58" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D58" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E58" s="4">
         <f>B58*C58/D58</f>
@@ -1719,17 +1716,17 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>75</v>
+      <c r="A59" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D59" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E59" s="4">
         <f>B59*C59/D59</f>
@@ -1738,16 +1735,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="C60" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D60" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E60" s="4">
         <f>B60*C60/D60</f>
@@ -1756,7 +1753,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
@@ -1773,8 +1770,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="6" t="s">
-        <v>62</v>
+      <c r="A62" t="s">
+        <v>42</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -1792,13 +1789,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>35</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
       </c>
       <c r="C63" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D63" s="1">
         <v>3</v>
@@ -1809,14 +1806,14 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>48</v>
+      <c r="A64" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
       </c>
       <c r="C64" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1">
         <v>3</v>
@@ -1828,7 +1825,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
@@ -1837,7 +1834,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E65" s="4">
         <f>B65*C65/D65</f>
@@ -1846,16 +1843,16 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
       </c>
       <c r="C66" s="1">
+        <v>4</v>
+      </c>
+      <c r="D66" s="1">
         <v>5</v>
-      </c>
-      <c r="D66" s="1">
-        <v>4</v>
       </c>
       <c r="E66" s="4">
         <f>B66*C66/D66</f>
@@ -1864,13 +1861,13 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
       </c>
       <c r="C67" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1">
         <v>4</v>
@@ -1881,14 +1878,14 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="2" t="s">
-        <v>12</v>
+      <c r="A68" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
       </c>
       <c r="C68" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D68" s="1">
         <v>4</v>
@@ -1900,13 +1897,13 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
       </c>
       <c r="C69" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D69" s="1">
         <v>4</v>
@@ -1918,7 +1915,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -1935,8 +1932,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
-        <v>43</v>
+      <c r="A71" t="s">
+        <v>61</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
@@ -1954,16 +1951,16 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
       </c>
       <c r="C72" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D72" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E72" s="4">
         <f>B72*C72/D72</f>
@@ -1972,16 +1969,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
       </c>
       <c r="C73" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D73" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E73" s="4">
         <f>B73*C73/D73</f>
@@ -1989,14 +1986,14 @@
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>61</v>
+      <c r="A74" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
       </c>
       <c r="C74" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" s="1">
         <v>4</v>
@@ -2007,49 +2004,31 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="3" t="s">
-        <v>18</v>
+      <c r="A75" t="s">
+        <v>69</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
       </c>
       <c r="C75" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D75" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E75" s="4">
         <f>B75*C75/D75</f>
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>46</v>
-      </c>
-      <c r="B76" s="1">
-        <v>0</v>
-      </c>
-      <c r="C76" s="1">
-        <v>4</v>
-      </c>
-      <c r="D76" s="1">
-        <v>5</v>
-      </c>
-      <c r="E76" s="4">
-        <f>B76*C76/D76</f>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E12" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E76">
-      <sortCondition descending="1" ref="E1:E12"/>
+  <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E75">
+      <sortCondition descending="1" ref="E1:E11"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E11">
-    <sortCondition descending="1" ref="E3:E11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E10">
+    <sortCondition descending="1" ref="E3:E10"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="colorScale" priority="3">
@@ -2063,7 +2042,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D47">
+  <conditionalFormatting sqref="D34:D46">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -2073,8 +2052,28 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32:C47">
+  <conditionalFormatting sqref="C31:C46">
     <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2084,7 +2083,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2094,7 +2093,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2104,7 +2103,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2114,7 +2113,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2124,7 +2123,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2134,7 +2133,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2144,7 +2143,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2154,7 +2153,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2164,7 +2163,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2174,7 +2173,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2184,7 +2183,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2194,7 +2193,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2204,7 +2203,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2214,7 +2213,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2224,26 +2223,6 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF5A8AC6"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="13">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -2295,8 +2274,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D36">
-    <cfRule type="colorScale" priority="87">
+  <conditionalFormatting sqref="D3:D35">
+    <cfRule type="colorScale" priority="112">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2305,8 +2284,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C31">
-    <cfRule type="colorScale" priority="89">
+  <conditionalFormatting sqref="C3:C30">
+    <cfRule type="colorScale" priority="114">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2315,8 +2294,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B76">
-    <cfRule type="colorScale" priority="91">
+  <conditionalFormatting sqref="B3:B75">
+    <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2326,7 +2305,7 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="92">
+    <cfRule type="colorScale" priority="117">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2335,8 +2314,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E47">
-    <cfRule type="colorScale" priority="95">
+  <conditionalFormatting sqref="E2:E46">
+    <cfRule type="colorScale" priority="120">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2347,8 +2326,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C47">
-    <cfRule type="colorScale" priority="97">
+  <conditionalFormatting sqref="C3:C46">
+    <cfRule type="colorScale" priority="122">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2357,8 +2336,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D47">
-    <cfRule type="colorScale" priority="99">
+  <conditionalFormatting sqref="D3:D46">
+    <cfRule type="colorScale" priority="124">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
Load from correct folders
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A362878-CE4F-4787-935D-DC2442F0978B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFA089F-752D-4942-B82D-F8996917C747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Name</t>
   </si>
@@ -276,7 +276,13 @@
     <t>Generate graphs automatically</t>
   </si>
   <si>
-    <t>Open files from specific folders (gui issue)</t>
+    <t>Update graphs more often</t>
+  </si>
+  <si>
+    <t>Autoprofile control loops</t>
+  </si>
+  <si>
+    <t>Open files from specific folders</t>
   </si>
 </sst>
 </file>
@@ -660,7 +666,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
@@ -730,7 +736,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
@@ -748,7 +754,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -766,43 +772,43 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="4">
         <f>B6*C6/D6</f>
-        <v>1.6666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="4">
         <f>B7*C7/D7</f>
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>66</v>
+      <c r="A8" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
@@ -811,34 +817,34 @@
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4">
         <f>B8*C8/D8</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>77</v>
+      <c r="A9" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="4">
         <f>B9*C9/D9</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
+      <c r="A10" t="s">
+        <v>64</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -855,8 +861,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
-        <v>29</v>
+      <c r="A11" t="s">
+        <v>80</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -865,47 +871,47 @@
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11" s="4">
         <f>B11*C11/D11</f>
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12" s="4">
         <f>B12*C12/D12</f>
-        <v>0.66666666666666663</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="B13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E13" s="4">
         <f>B13*C13/D13</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1108,7 +1114,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1126,7 +1132,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -1144,7 +1150,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1162,7 +1168,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1180,16 +1186,16 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
       </c>
       <c r="C29" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="4">
         <f>B29*C29/D29</f>
@@ -1198,7 +1204,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1216,7 +1222,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -1234,16 +1240,16 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
       </c>
       <c r="C32" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" s="4">
         <f>B32*C32/D32</f>
@@ -1252,16 +1258,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D33" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="4">
         <f>B33*C33/D33</f>
@@ -1269,8 +1275,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>23</v>
+      <c r="A34" t="s">
+        <v>78</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -1288,7 +1294,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -1305,8 +1311,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>41</v>
+      <c r="A36" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -1323,17 +1329,17 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="3" t="s">
-        <v>44</v>
+      <c r="A37" t="s">
+        <v>56</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
       </c>
       <c r="C37" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E37" s="4">
         <f>B37*C37/D37</f>
@@ -1341,14 +1347,14 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>58</v>
+      <c r="A38" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
       </c>
       <c r="C38" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38" s="1">
         <v>2</v>
@@ -1360,16 +1366,16 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
       </c>
       <c r="C39" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D39" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E39" s="4">
         <f>B39*C39/D39</f>
@@ -1377,8 +1383,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="3" t="s">
-        <v>33</v>
+      <c r="A40" t="s">
+        <v>58</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
@@ -1395,8 +1401,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>16</v>
+      <c r="A41" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
@@ -1414,7 +1420,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
@@ -1431,17 +1437,17 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
-        <v>49</v>
+      <c r="A43" t="s">
+        <v>16</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
       </c>
       <c r="C43" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E43" s="4">
         <f>B43*C43/D43</f>
@@ -1449,17 +1455,17 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
-        <v>31</v>
+      <c r="A44" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
       </c>
       <c r="C44" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E44" s="4">
         <f>B44*C44/D44</f>
@@ -1468,7 +1474,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -1486,7 +1492,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
@@ -1504,7 +1510,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
@@ -1522,7 +1528,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -1540,7 +1546,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1557,8 +1563,8 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>21</v>
+      <c r="A50" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -1575,8 +1581,8 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>8</v>
+      <c r="A51" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -1594,7 +1600,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -1612,7 +1618,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1629,8 +1635,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="3" t="s">
-        <v>47</v>
+      <c r="A54" t="s">
+        <v>11</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -1647,8 +1653,8 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="5" t="s">
-        <v>13</v>
+      <c r="A55" t="s">
+        <v>40</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -1665,17 +1671,17 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>17</v>
+      <c r="A56" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
       </c>
       <c r="C56" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D56" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E56" s="4">
         <f>B56*C56/D56</f>
@@ -1683,17 +1689,17 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>1</v>
+      <c r="A57" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
       </c>
       <c r="C57" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D57" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E57" s="4">
         <f>B57*C57/D57</f>
@@ -1702,16 +1708,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D58" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E58" s="4">
         <f>B58*C58/D58</f>
@@ -1720,16 +1726,16 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D59" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E59" s="4">
         <f>B59*C59/D59</f>
@@ -1738,16 +1744,16 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="C60" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D60" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E60" s="4">
         <f>B60*C60/D60</f>
@@ -1756,16 +1762,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
       </c>
       <c r="C61" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D61" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E61" s="4">
         <f>B61*C61/D61</f>
@@ -1774,7 +1780,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
@@ -1791,8 +1797,8 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="6" t="s">
-        <v>62</v>
+      <c r="A63" t="s">
+        <v>42</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
@@ -1809,17 +1815,17 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
-        <v>12</v>
+      <c r="A64" t="s">
+        <v>35</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
       </c>
       <c r="C64" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D64" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E64" s="4">
         <f>B64*C64/D64</f>
@@ -1827,17 +1833,17 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>19</v>
+      <c r="A65" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
       </c>
       <c r="C65" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D65" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E65" s="4">
         <f>B65*C65/D65</f>
@@ -1845,17 +1851,17 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="3" t="s">
-        <v>18</v>
+      <c r="A66" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
       </c>
       <c r="C66" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D66" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E66" s="4">
         <f>B66*C66/D66</f>
@@ -1864,7 +1870,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
@@ -1873,7 +1879,7 @@
         <v>4</v>
       </c>
       <c r="D67" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E67" s="4">
         <f>B67*C67/D67</f>
@@ -1881,17 +1887,17 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>65</v>
+      <c r="A68" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
       </c>
       <c r="C68" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D68" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E68" s="4">
         <f>B68*C68/D68</f>
@@ -1899,17 +1905,17 @@
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" s="3" t="s">
-        <v>43</v>
+      <c r="A69" t="s">
+        <v>46</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
       </c>
       <c r="C69" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D69" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E69" s="4">
         <f>B69*C69/D69</f>
@@ -1918,7 +1924,7 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
@@ -1935,8 +1941,8 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>20</v>
+      <c r="A71" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
@@ -1954,7 +1960,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -1972,16 +1978,16 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
       </c>
       <c r="C73" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D73" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E73" s="4">
         <f>B73*C73/D73</f>
@@ -1990,16 +1996,16 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
       </c>
       <c r="C74" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D74" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E74" s="4">
         <f>B74*C74/D74</f>
@@ -2007,8 +2013,8 @@
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
-        <v>74</v>
+      <c r="A75" t="s">
+        <v>60</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
@@ -2017,7 +2023,7 @@
         <v>2</v>
       </c>
       <c r="D75" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E75" s="4">
         <f>B75*C75/D75</f>
@@ -2026,13 +2032,13 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
       </c>
       <c r="C76" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D76" s="1">
         <v>3</v>
@@ -2042,9 +2048,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1">
+        <v>2</v>
+      </c>
+      <c r="D77" s="1">
+        <v>4</v>
+      </c>
+      <c r="E77" s="4">
+        <f>B77*C77/D77</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" s="1">
+        <v>0</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1</v>
+      </c>
+      <c r="D78" s="1">
+        <v>3</v>
+      </c>
+      <c r="E78" s="4">
+        <f>B78*C78/D78</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E76">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
       <sortCondition descending="1" ref="E1:E11"/>
     </sortState>
   </autoFilter>
@@ -2315,7 +2357,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B76">
+  <conditionalFormatting sqref="B3:B78">
     <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
PID progress and pressure test
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFA089F-752D-4942-B82D-F8996917C747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CACCCC-595F-453A-99DE-C2B1311BFA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -283,6 +283,12 @@
   </si>
   <si>
     <t>Open files from specific folders</t>
+  </si>
+  <si>
+    <t>Change explicit list access to using .get()</t>
+  </si>
+  <si>
+    <t>Investigate graph issue: redundant append</t>
   </si>
 </sst>
 </file>
@@ -666,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,97 +742,97 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4">
         <f>B4*C4/D4</f>
-        <v>1.6666666666666667</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="4">
         <f>B5*C5/D5</f>
-        <v>1.6666666666666667</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D6" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="4">
         <f>B6*C6/D6</f>
-        <v>1</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="4">
         <f>B7*C7/D7</f>
-        <v>1</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>28</v>
+      <c r="A8" t="s">
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E8" s="4">
         <f>B8*C8/D8</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>29</v>
+      <c r="A9" t="s">
+        <v>66</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -835,34 +841,34 @@
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E9" s="4">
         <f>B9*C9/D9</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="4">
         <f>B10*C10/D10</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>80</v>
+      <c r="A11" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -871,88 +877,88 @@
         <v>2</v>
       </c>
       <c r="D11" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E11" s="4">
         <f>B11*C11/D11</f>
-        <v>0.5</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>51</v>
+      <c r="A12" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" s="4">
         <f>B12*C12/D12</f>
-        <v>0.2</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13" s="1">
         <v>3</v>
       </c>
       <c r="E13" s="4">
         <f>B13*C13/D13</f>
-        <v>0</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="B14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E14" s="4">
         <f>B14*C14/D14</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
         <v>5</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
       </c>
       <c r="E15" s="4">
         <f>B15*C15/D15</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -970,7 +976,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -988,7 +994,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1006,13 +1012,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
       </c>
       <c r="C19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -1024,13 +1030,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1042,7 +1048,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1060,7 +1066,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1078,7 +1084,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -1095,8 +1101,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>30</v>
+      <c r="A24" t="s">
+        <v>4</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1114,13 +1120,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
@@ -1131,14 +1137,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>53</v>
+      <c r="A26" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1150,7 +1156,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1168,7 +1174,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>53</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1186,7 +1192,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1204,16 +1210,16 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
       </c>
       <c r="C30" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="4">
         <f>B30*C30/D30</f>
@@ -1222,16 +1228,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D31" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E31" s="4">
         <f>B31*C31/D31</f>
@@ -1240,7 +1246,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1258,16 +1264,16 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
       </c>
       <c r="C33" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D33" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="4">
         <f>B33*C33/D33</f>
@@ -1276,13 +1282,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
@@ -1294,16 +1300,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="4">
         <f>B35*C35/D35</f>
@@ -1311,8 +1317,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="2" t="s">
-        <v>23</v>
+      <c r="A36" t="s">
+        <v>78</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -1330,7 +1336,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -1347,8 +1353,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="3" t="s">
-        <v>41</v>
+      <c r="A38" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -1365,17 +1371,17 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
-        <v>44</v>
+      <c r="A39" t="s">
+        <v>56</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
       </c>
       <c r="C39" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D39" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E39" s="4">
         <f>B39*C39/D39</f>
@@ -1383,14 +1389,14 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>58</v>
+      <c r="A40" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B40" s="1">
         <v>0</v>
       </c>
       <c r="C40" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D40" s="1">
         <v>2</v>
@@ -1401,17 +1407,17 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="3" t="s">
-        <v>39</v>
+      <c r="A41" t="s">
+        <v>81</v>
       </c>
       <c r="B41" s="1">
         <v>0</v>
       </c>
       <c r="C41" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D41" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" s="4">
         <f>B41*C41/D41</f>
@@ -1420,16 +1426,16 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B42" s="1">
         <v>0</v>
       </c>
       <c r="C42" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D42" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E42" s="4">
         <f>B42*C42/D42</f>
@@ -1438,7 +1444,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -1456,7 +1462,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -1473,17 +1479,17 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="2" t="s">
-        <v>49</v>
+      <c r="A45" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
       </c>
       <c r="C45" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D45" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E45" s="4">
         <f>B45*C45/D45</f>
@@ -1491,17 +1497,17 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
-        <v>31</v>
+      <c r="A46" t="s">
+        <v>16</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
       </c>
       <c r="C46" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D46" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E46" s="4">
         <f>B46*C46/D46</f>
@@ -1509,17 +1515,17 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="2" t="s">
-        <v>26</v>
+      <c r="A47" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="B47" s="1">
         <v>0</v>
       </c>
       <c r="C47" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" s="4">
         <f>B47*C47/D47</f>
@@ -1528,7 +1534,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -1546,7 +1552,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1564,7 +1570,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B50" s="1">
         <v>0</v>
@@ -1582,7 +1588,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -1599,8 +1605,8 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>21</v>
+      <c r="A52" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B52" s="1">
         <v>0</v>
@@ -1617,8 +1623,8 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>8</v>
+      <c r="A53" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B53" s="1">
         <v>0</v>
@@ -1635,8 +1641,8 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>11</v>
+      <c r="A54" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B54" s="1">
         <v>0</v>
@@ -1654,7 +1660,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B55" s="1">
         <v>0</v>
@@ -1671,8 +1677,8 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="3" t="s">
-        <v>47</v>
+      <c r="A56" t="s">
+        <v>8</v>
       </c>
       <c r="B56" s="1">
         <v>0</v>
@@ -1689,8 +1695,8 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
-        <v>13</v>
+      <c r="A57" t="s">
+        <v>11</v>
       </c>
       <c r="B57" s="1">
         <v>0</v>
@@ -1708,16 +1714,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B58" s="1">
         <v>0</v>
       </c>
       <c r="C58" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D58" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E58" s="4">
         <f>B58*C58/D58</f>
@@ -1725,17 +1731,17 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>1</v>
+      <c r="A59" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="B59" s="1">
         <v>0</v>
       </c>
       <c r="C59" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D59" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E59" s="4">
         <f>B59*C59/D59</f>
@@ -1743,17 +1749,17 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>9</v>
+      <c r="A60" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B60" s="1">
         <v>0</v>
       </c>
       <c r="C60" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D60" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E60" s="4">
         <f>B60*C60/D60</f>
@@ -1762,16 +1768,16 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>17</v>
       </c>
       <c r="B61" s="1">
         <v>0</v>
       </c>
       <c r="C61" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D61" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E61" s="4">
         <f>B61*C61/D61</f>
@@ -1780,16 +1786,16 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="B62" s="1">
         <v>0</v>
       </c>
       <c r="C62" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D62" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E62" s="4">
         <f>B62*C62/D62</f>
@@ -1798,16 +1804,16 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="B63" s="1">
         <v>0</v>
       </c>
       <c r="C63" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E63" s="4">
         <f>B63*C63/D63</f>
@@ -1816,7 +1822,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B64" s="1">
         <v>0</v>
@@ -1833,8 +1839,8 @@
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" s="6" t="s">
-        <v>62</v>
+      <c r="A65" t="s">
+        <v>42</v>
       </c>
       <c r="B65" s="1">
         <v>0</v>
@@ -1851,17 +1857,17 @@
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>12</v>
+      <c r="A66" t="s">
+        <v>35</v>
       </c>
       <c r="B66" s="1">
         <v>0</v>
       </c>
       <c r="C66" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D66" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E66" s="4">
         <f>B66*C66/D66</f>
@@ -1869,17 +1875,17 @@
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>19</v>
+      <c r="A67" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="B67" s="1">
         <v>0</v>
       </c>
       <c r="C67" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E67" s="4">
         <f>B67*C67/D67</f>
@@ -1887,17 +1893,17 @@
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" s="3" t="s">
-        <v>18</v>
+      <c r="A68" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B68" s="1">
         <v>0</v>
       </c>
       <c r="C68" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D68" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E68" s="4">
         <f>B68*C68/D68</f>
@@ -1906,7 +1912,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B69" s="1">
         <v>0</v>
@@ -1915,7 +1921,7 @@
         <v>4</v>
       </c>
       <c r="D69" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E69" s="4">
         <f>B69*C69/D69</f>
@@ -1923,17 +1929,17 @@
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>65</v>
+      <c r="A70" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="B70" s="1">
         <v>0</v>
       </c>
       <c r="C70" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D70" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E70" s="4">
         <f>B70*C70/D70</f>
@@ -1941,17 +1947,17 @@
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" s="3" t="s">
-        <v>43</v>
+      <c r="A71" t="s">
+        <v>46</v>
       </c>
       <c r="B71" s="1">
         <v>0</v>
       </c>
       <c r="C71" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D71" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E71" s="4">
         <f>B71*C71/D71</f>
@@ -1960,7 +1966,7 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="B72" s="1">
         <v>0</v>
@@ -1977,8 +1983,8 @@
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>20</v>
+      <c r="A73" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="B73" s="1">
         <v>0</v>
@@ -1996,7 +2002,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="B74" s="1">
         <v>0</v>
@@ -2014,16 +2020,16 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="B75" s="1">
         <v>0</v>
       </c>
       <c r="C75" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D75" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E75" s="4">
         <f>B75*C75/D75</f>
@@ -2032,16 +2038,16 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B76" s="1">
         <v>0</v>
       </c>
       <c r="C76" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D76" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E76" s="4">
         <f>B76*C76/D76</f>
@@ -2049,8 +2055,8 @@
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" s="2" t="s">
-        <v>74</v>
+      <c r="A77" t="s">
+        <v>60</v>
       </c>
       <c r="B77" s="1">
         <v>0</v>
@@ -2059,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="D77" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E77" s="4">
         <f>B77*C77/D77</f>
@@ -2068,13 +2074,13 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B78" s="1">
         <v>0</v>
       </c>
       <c r="C78" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D78" s="1">
         <v>3</v>
@@ -2084,9 +2090,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79" s="1">
+        <v>0</v>
+      </c>
+      <c r="C79" s="1">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1">
+        <v>4</v>
+      </c>
+      <c r="E79" s="4">
+        <f>B79*C79/D79</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="1">
+        <v>0</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1">
+        <v>3</v>
+      </c>
+      <c r="E80" s="4">
+        <f>B80*C80/D80</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E11" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E78">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E80">
       <sortCondition descending="1" ref="E1:E11"/>
     </sortState>
   </autoFilter>
@@ -2357,7 +2399,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B78">
+  <conditionalFormatting sqref="B3:B79">
     <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Replaced direct indexing in most instances with .get(), and updated all job files so that they should work in current build.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCC5E22-34D8-4C49-8FD4-9AA2789740AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DAA9B4-EAFC-40AE-9BDE-2FAF465E4AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -678,7 +678,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F81" sqref="F81"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,25 +763,25 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="4">
         <f>B5*C5/D5</f>
-        <v>2</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -799,34 +799,34 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E7" s="4">
         <f>B7*C7/D7</f>
-        <v>1.6666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4">
         <f>B8*C8/D8</f>
@@ -835,16 +835,16 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
       </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D9" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="4">
         <f>B9*C9/D9</f>
@@ -852,26 +852,26 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>77</v>
+      <c r="A10" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1">
         <v>3</v>
       </c>
       <c r="E10" s="4">
         <f>B10*C10/D10</f>
-        <v>1</v>
+        <v>0.66666666666666663</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
@@ -888,8 +888,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>29</v>
+      <c r="A12" t="s">
+        <v>64</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
@@ -907,25 +907,25 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1">
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E13" s="4">
         <f>B13*C13/D13</f>
-        <v>0.66666666666666663</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
@@ -943,25 +943,25 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E15" s="4">
         <f>B15*C15/D15</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="B19" s="1">
         <v>0</v>
@@ -1033,13 +1033,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
         <v>1</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="B23" s="1">
         <v>0</v>
@@ -1105,7 +1105,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1">
         <v>0</v>
@@ -1122,8 +1122,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>54</v>
+      <c r="A25" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1140,14 +1140,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>30</v>
+      <c r="A26" t="s">
+        <v>79</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
@@ -1159,7 +1159,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -1177,7 +1177,7 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1231,16 +1231,16 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
       </c>
       <c r="C31" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E31" s="4">
         <f>B31*C31/D31</f>
@@ -1249,7 +1249,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -1285,16 +1285,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
       </c>
       <c r="C34" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="4">
         <f>B34*C34/D34</f>
@@ -1303,16 +1303,16 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
       </c>
       <c r="C35" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="4">
         <f>B35*C35/D35</f>
@@ -2420,7 +2420,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B80">
+  <conditionalFormatting sqref="B3:B81">
     <cfRule type="colorScale" priority="116">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Assured changed to check time after values.
</commit_message>
<xml_diff>
--- a/hs-logger_priorities.xlsx
+++ b/hs-logger_priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b.sherson.CI\PycharmProjects\hs-logger\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DAA9B4-EAFC-40AE-9BDE-2FAF465E4AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52D6C0B2-B75D-45FB-BB3F-D92AC957A687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14655" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -678,7 +678,7 @@
   <dimension ref="A1:E81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -727,7 +727,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -745,25 +745,25 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E4" s="4">
         <f>B4*C4/D4</f>
-        <v>3</v>
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -781,20 +781,20 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
       <c r="C6" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="4">
         <f>B6*C6/D6</f>
-        <v>1.6666666666666667</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>